<commit_message>
Added and updated images and data imports
</commit_message>
<xml_diff>
--- a/resources/data-imports/items.xlsx
+++ b/resources/data-imports/items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="433">
   <si>
     <t>item_suffix_id</t>
   </si>
@@ -1299,6 +1299,21 @@
   </si>
   <si>
     <t>Allows you to enchant easily.</t>
+  </si>
+  <si>
+    <t>Astral Ring</t>
+  </si>
+  <si>
+    <t>Fighters Strength</t>
+  </si>
+  <si>
+    <t>Natures Balancing Bliss</t>
+  </si>
+  <si>
+    <t>Spell Crafters Blood</t>
+  </si>
+  <si>
+    <t>Weapon Crafter Spell</t>
   </si>
 </sst>
 </file>
@@ -1637,7 +1652,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA189"/>
+  <dimension ref="A1:AA194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1645,8 +1660,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="35.2771" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="16.424561" bestFit="true" customWidth="true" style="0"/>
@@ -2061,6 +2076,9 @@
       <c r="F11" t="s">
         <v>55</v>
       </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
       <c r="J11">
         <v>6</v>
       </c>
@@ -9058,6 +9076,226 @@
       </c>
       <c r="AA189">
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="190" spans="1:27">
+      <c r="B190" t="s">
+        <v>428</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+      <c r="D190" t="s">
+        <v>323</v>
+      </c>
+      <c r="E190" t="s">
+        <v>306</v>
+      </c>
+      <c r="F190" t="s">
+        <v>324</v>
+      </c>
+      <c r="H190">
+        <v>85</v>
+      </c>
+      <c r="K190">
+        <v>18000</v>
+      </c>
+      <c r="U190">
+        <v>1</v>
+      </c>
+      <c r="V190">
+        <v>36</v>
+      </c>
+      <c r="W190">
+        <v>70</v>
+      </c>
+      <c r="X190" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="191" spans="1:27">
+      <c r="A191" t="s">
+        <v>429</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191" t="s">
+        <v>128</v>
+      </c>
+      <c r="E191" t="s">
+        <v>47</v>
+      </c>
+      <c r="F191" t="s">
+        <v>129</v>
+      </c>
+      <c r="G191" t="s">
+        <v>47</v>
+      </c>
+      <c r="J191">
+        <v>30</v>
+      </c>
+      <c r="K191">
+        <v>945</v>
+      </c>
+      <c r="O191">
+        <v>0.06</v>
+      </c>
+      <c r="P191">
+        <v>0.06</v>
+      </c>
+      <c r="Q191">
+        <v>0.06</v>
+      </c>
+      <c r="R191">
+        <v>0.06</v>
+      </c>
+      <c r="S191">
+        <v>0.06</v>
+      </c>
+      <c r="U191">
+        <v>1</v>
+      </c>
+      <c r="V191">
+        <v>24</v>
+      </c>
+      <c r="W191">
+        <v>40</v>
+      </c>
+      <c r="X191" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="192" spans="1:27">
+      <c r="A192" t="s">
+        <v>430</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="D192" t="s">
+        <v>30</v>
+      </c>
+      <c r="E192" t="s">
+        <v>31</v>
+      </c>
+      <c r="F192" t="s">
+        <v>32</v>
+      </c>
+      <c r="G192" t="s">
+        <v>31</v>
+      </c>
+      <c r="J192">
+        <v>4</v>
+      </c>
+      <c r="K192">
+        <v>10</v>
+      </c>
+      <c r="U192">
+        <v>1</v>
+      </c>
+      <c r="V192">
+        <v>1</v>
+      </c>
+      <c r="W192">
+        <v>5</v>
+      </c>
+      <c r="X192" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="193" spans="1:27">
+      <c r="B193" t="s">
+        <v>431</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+      <c r="D193" t="s">
+        <v>100</v>
+      </c>
+      <c r="E193" t="s">
+        <v>28</v>
+      </c>
+      <c r="F193" t="s">
+        <v>101</v>
+      </c>
+      <c r="H193">
+        <v>80</v>
+      </c>
+      <c r="K193">
+        <v>750</v>
+      </c>
+      <c r="O193">
+        <v>0.18</v>
+      </c>
+      <c r="P193">
+        <v>0.18</v>
+      </c>
+      <c r="Q193">
+        <v>0.18</v>
+      </c>
+      <c r="R193">
+        <v>0.18</v>
+      </c>
+      <c r="S193">
+        <v>0.18</v>
+      </c>
+      <c r="U193">
+        <v>1</v>
+      </c>
+      <c r="V193">
+        <v>18</v>
+      </c>
+      <c r="W193">
+        <v>36</v>
+      </c>
+      <c r="X193" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="194" spans="1:27">
+      <c r="B194" t="s">
+        <v>432</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194" t="s">
+        <v>297</v>
+      </c>
+      <c r="E194" t="s">
+        <v>273</v>
+      </c>
+      <c r="F194" t="s">
+        <v>298</v>
+      </c>
+      <c r="H194">
+        <v>75</v>
+      </c>
+      <c r="K194">
+        <v>133000</v>
+      </c>
+      <c r="L194">
+        <v>0.25</v>
+      </c>
+      <c r="M194">
+        <v>0.25</v>
+      </c>
+      <c r="N194">
+        <v>0.25</v>
+      </c>
+      <c r="U194">
+        <v>1</v>
+      </c>
+      <c r="V194">
+        <v>50</v>
+      </c>
+      <c r="W194">
+        <v>100</v>
+      </c>
+      <c r="X194" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got the map images into place
</commit_message>
<xml_diff>
--- a/resources/data-imports/items.xlsx
+++ b/resources/data-imports/items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="454">
   <si>
     <t>item_suffix_id</t>
   </si>
@@ -1353,6 +1353,30 @@
   </si>
   <si>
     <t>Archers Bane</t>
+  </si>
+  <si>
+    <t>Eye For Gold</t>
+  </si>
+  <si>
+    <t>Sinister Dance</t>
+  </si>
+  <si>
+    <t>Blood Lust</t>
+  </si>
+  <si>
+    <t>Dancers Moves</t>
+  </si>
+  <si>
+    <t>Enchantress Luck</t>
+  </si>
+  <si>
+    <t>Mages Inspiration</t>
+  </si>
+  <si>
+    <t>Deaths Accuracy</t>
+  </si>
+  <si>
+    <t>Hawk Eye</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1715,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA212"/>
+  <dimension ref="A1:AA242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2616,7 +2640,7 @@
         <v>12</v>
       </c>
       <c r="X24" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -10156,6 +10180,1407 @@
         <v>180</v>
       </c>
       <c r="X212" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="213" spans="1:27">
+      <c r="B213" t="s">
+        <v>446</v>
+      </c>
+      <c r="C213">
+        <v>1</v>
+      </c>
+      <c r="D213" t="s">
+        <v>212</v>
+      </c>
+      <c r="E213" t="s">
+        <v>31</v>
+      </c>
+      <c r="F213" t="s">
+        <v>213</v>
+      </c>
+      <c r="G213" t="s">
+        <v>31</v>
+      </c>
+      <c r="J213">
+        <v>190</v>
+      </c>
+      <c r="K213">
+        <v>125000</v>
+      </c>
+      <c r="O213">
+        <v>0.36</v>
+      </c>
+      <c r="P213">
+        <v>0.36</v>
+      </c>
+      <c r="Q213">
+        <v>0.36</v>
+      </c>
+      <c r="R213">
+        <v>0.36</v>
+      </c>
+      <c r="S213">
+        <v>0.36</v>
+      </c>
+      <c r="U213">
+        <v>1</v>
+      </c>
+      <c r="V213">
+        <v>50</v>
+      </c>
+      <c r="W213">
+        <v>100</v>
+      </c>
+      <c r="X213" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="214" spans="1:27">
+      <c r="A214" t="s">
+        <v>440</v>
+      </c>
+      <c r="C214">
+        <v>1</v>
+      </c>
+      <c r="D214" t="s">
+        <v>52</v>
+      </c>
+      <c r="E214" t="s">
+        <v>28</v>
+      </c>
+      <c r="F214" t="s">
+        <v>53</v>
+      </c>
+      <c r="H214">
+        <v>8</v>
+      </c>
+      <c r="K214">
+        <v>50</v>
+      </c>
+      <c r="O214">
+        <v>0.05</v>
+      </c>
+      <c r="P214">
+        <v>0.05</v>
+      </c>
+      <c r="Q214">
+        <v>0.05</v>
+      </c>
+      <c r="R214">
+        <v>0.05</v>
+      </c>
+      <c r="S214">
+        <v>0.05</v>
+      </c>
+      <c r="U214">
+        <v>1</v>
+      </c>
+      <c r="V214">
+        <v>3</v>
+      </c>
+      <c r="W214">
+        <v>8</v>
+      </c>
+      <c r="X214" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="215" spans="1:27">
+      <c r="B215" t="s">
+        <v>447</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
+      </c>
+      <c r="D215" t="s">
+        <v>198</v>
+      </c>
+      <c r="E215" t="s">
+        <v>31</v>
+      </c>
+      <c r="F215" t="s">
+        <v>199</v>
+      </c>
+      <c r="G215" t="s">
+        <v>31</v>
+      </c>
+      <c r="J215">
+        <v>170</v>
+      </c>
+      <c r="K215">
+        <v>48000</v>
+      </c>
+      <c r="O215">
+        <v>0.33</v>
+      </c>
+      <c r="P215">
+        <v>0.33</v>
+      </c>
+      <c r="Q215">
+        <v>0.33</v>
+      </c>
+      <c r="R215">
+        <v>0.33</v>
+      </c>
+      <c r="S215">
+        <v>0.33</v>
+      </c>
+      <c r="U215">
+        <v>1</v>
+      </c>
+      <c r="V215">
+        <v>43</v>
+      </c>
+      <c r="W215">
+        <v>78</v>
+      </c>
+      <c r="X215" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="216" spans="1:27">
+      <c r="A216" t="s">
+        <v>448</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216" t="s">
+        <v>52</v>
+      </c>
+      <c r="E216" t="s">
+        <v>28</v>
+      </c>
+      <c r="F216" t="s">
+        <v>53</v>
+      </c>
+      <c r="H216">
+        <v>8</v>
+      </c>
+      <c r="K216">
+        <v>50</v>
+      </c>
+      <c r="O216">
+        <v>0.05</v>
+      </c>
+      <c r="P216">
+        <v>0.05</v>
+      </c>
+      <c r="Q216">
+        <v>0.05</v>
+      </c>
+      <c r="R216">
+        <v>0.05</v>
+      </c>
+      <c r="S216">
+        <v>0.05</v>
+      </c>
+      <c r="U216">
+        <v>1</v>
+      </c>
+      <c r="V216">
+        <v>3</v>
+      </c>
+      <c r="W216">
+        <v>8</v>
+      </c>
+      <c r="X216" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="217" spans="1:27">
+      <c r="A217" t="s">
+        <v>448</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+      <c r="D217" t="s">
+        <v>27</v>
+      </c>
+      <c r="E217" t="s">
+        <v>28</v>
+      </c>
+      <c r="F217" t="s">
+        <v>29</v>
+      </c>
+      <c r="H217">
+        <v>4</v>
+      </c>
+      <c r="K217">
+        <v>10</v>
+      </c>
+      <c r="U217">
+        <v>1</v>
+      </c>
+      <c r="V217">
+        <v>1</v>
+      </c>
+      <c r="W217">
+        <v>5</v>
+      </c>
+      <c r="X217" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="218" spans="1:27">
+      <c r="A218" t="s">
+        <v>429</v>
+      </c>
+      <c r="C218">
+        <v>1</v>
+      </c>
+      <c r="D218" t="s">
+        <v>27</v>
+      </c>
+      <c r="E218" t="s">
+        <v>28</v>
+      </c>
+      <c r="F218" t="s">
+        <v>29</v>
+      </c>
+      <c r="H218">
+        <v>4</v>
+      </c>
+      <c r="K218">
+        <v>10</v>
+      </c>
+      <c r="U218">
+        <v>1</v>
+      </c>
+      <c r="V218">
+        <v>1</v>
+      </c>
+      <c r="W218">
+        <v>5</v>
+      </c>
+      <c r="X218" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="219" spans="1:27">
+      <c r="A219" t="s">
+        <v>445</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+      <c r="D219" t="s">
+        <v>27</v>
+      </c>
+      <c r="E219" t="s">
+        <v>28</v>
+      </c>
+      <c r="F219" t="s">
+        <v>29</v>
+      </c>
+      <c r="H219">
+        <v>4</v>
+      </c>
+      <c r="K219">
+        <v>10</v>
+      </c>
+      <c r="U219">
+        <v>1</v>
+      </c>
+      <c r="V219">
+        <v>1</v>
+      </c>
+      <c r="W219">
+        <v>5</v>
+      </c>
+      <c r="X219" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="220" spans="1:27">
+      <c r="B220" t="s">
+        <v>449</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+      <c r="D220" t="s">
+        <v>102</v>
+      </c>
+      <c r="E220" t="s">
+        <v>31</v>
+      </c>
+      <c r="F220" t="s">
+        <v>103</v>
+      </c>
+      <c r="G220" t="s">
+        <v>31</v>
+      </c>
+      <c r="J220">
+        <v>40</v>
+      </c>
+      <c r="K220">
+        <v>750</v>
+      </c>
+      <c r="O220">
+        <v>0.18</v>
+      </c>
+      <c r="P220">
+        <v>0.18</v>
+      </c>
+      <c r="Q220">
+        <v>0.18</v>
+      </c>
+      <c r="R220">
+        <v>0.18</v>
+      </c>
+      <c r="S220">
+        <v>0.18</v>
+      </c>
+      <c r="U220">
+        <v>1</v>
+      </c>
+      <c r="V220">
+        <v>18</v>
+      </c>
+      <c r="W220">
+        <v>36</v>
+      </c>
+      <c r="X220" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="221" spans="1:27">
+      <c r="A221" t="s">
+        <v>435</v>
+      </c>
+      <c r="B221" t="s">
+        <v>442</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
+      <c r="D221" t="s">
+        <v>256</v>
+      </c>
+      <c r="E221" t="s">
+        <v>28</v>
+      </c>
+      <c r="F221" t="s">
+        <v>257</v>
+      </c>
+      <c r="H221">
+        <v>450</v>
+      </c>
+      <c r="K221">
+        <v>1525000</v>
+      </c>
+      <c r="O221">
+        <v>0.37</v>
+      </c>
+      <c r="P221">
+        <v>0.37</v>
+      </c>
+      <c r="Q221">
+        <v>0.37</v>
+      </c>
+      <c r="R221">
+        <v>0.37</v>
+      </c>
+      <c r="S221">
+        <v>0.37</v>
+      </c>
+      <c r="U221">
+        <v>1</v>
+      </c>
+      <c r="V221">
+        <v>70</v>
+      </c>
+      <c r="W221">
+        <v>150</v>
+      </c>
+      <c r="X221" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="222" spans="1:27">
+      <c r="B222" t="s">
+        <v>446</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+      <c r="D222" t="s">
+        <v>366</v>
+      </c>
+      <c r="E222" t="s">
+        <v>340</v>
+      </c>
+      <c r="F222" t="s">
+        <v>367</v>
+      </c>
+      <c r="I222">
+        <v>260</v>
+      </c>
+      <c r="K222">
+        <v>320000</v>
+      </c>
+      <c r="U222">
+        <v>1</v>
+      </c>
+      <c r="V222">
+        <v>55</v>
+      </c>
+      <c r="W222">
+        <v>110</v>
+      </c>
+      <c r="X222" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="223" spans="1:27">
+      <c r="B223" t="s">
+        <v>450</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223" t="s">
+        <v>34</v>
+      </c>
+      <c r="E223" t="s">
+        <v>35</v>
+      </c>
+      <c r="F223" t="s">
+        <v>36</v>
+      </c>
+      <c r="J223">
+        <v>1</v>
+      </c>
+      <c r="K223">
+        <v>5</v>
+      </c>
+      <c r="U223">
+        <v>1</v>
+      </c>
+      <c r="V223">
+        <v>1</v>
+      </c>
+      <c r="W223">
+        <v>5</v>
+      </c>
+      <c r="X223" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="224" spans="1:27">
+      <c r="B224" t="s">
+        <v>450</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+      <c r="D224" t="s">
+        <v>56</v>
+      </c>
+      <c r="E224" t="s">
+        <v>35</v>
+      </c>
+      <c r="F224" t="s">
+        <v>57</v>
+      </c>
+      <c r="J224">
+        <v>3</v>
+      </c>
+      <c r="K224">
+        <v>60</v>
+      </c>
+      <c r="O224">
+        <v>0.02</v>
+      </c>
+      <c r="P224">
+        <v>0.02</v>
+      </c>
+      <c r="Q224">
+        <v>0.02</v>
+      </c>
+      <c r="R224">
+        <v>0.02</v>
+      </c>
+      <c r="S224">
+        <v>0.02</v>
+      </c>
+      <c r="U224">
+        <v>1</v>
+      </c>
+      <c r="V224">
+        <v>3</v>
+      </c>
+      <c r="W224">
+        <v>8</v>
+      </c>
+      <c r="X224" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="225" spans="1:27">
+      <c r="A225" t="s">
+        <v>451</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225" t="s">
+        <v>238</v>
+      </c>
+      <c r="E225" t="s">
+        <v>50</v>
+      </c>
+      <c r="F225" t="s">
+        <v>239</v>
+      </c>
+      <c r="J225">
+        <v>150</v>
+      </c>
+      <c r="K225">
+        <v>360000</v>
+      </c>
+      <c r="O225">
+        <v>0.18</v>
+      </c>
+      <c r="P225">
+        <v>0.18</v>
+      </c>
+      <c r="Q225">
+        <v>0.18</v>
+      </c>
+      <c r="R225">
+        <v>0.18</v>
+      </c>
+      <c r="S225">
+        <v>0.18</v>
+      </c>
+      <c r="U225">
+        <v>1</v>
+      </c>
+      <c r="V225">
+        <v>55</v>
+      </c>
+      <c r="W225">
+        <v>110</v>
+      </c>
+      <c r="X225" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="226" spans="1:27">
+      <c r="A226" t="s">
+        <v>444</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+      <c r="D226" t="s">
+        <v>64</v>
+      </c>
+      <c r="E226" t="s">
+        <v>47</v>
+      </c>
+      <c r="F226" t="s">
+        <v>65</v>
+      </c>
+      <c r="G226" t="s">
+        <v>47</v>
+      </c>
+      <c r="J226">
+        <v>3</v>
+      </c>
+      <c r="K226">
+        <v>55</v>
+      </c>
+      <c r="U226">
+        <v>1</v>
+      </c>
+      <c r="V226">
+        <v>3</v>
+      </c>
+      <c r="W226">
+        <v>8</v>
+      </c>
+      <c r="X226" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="227" spans="1:27">
+      <c r="B227" t="s">
+        <v>442</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227" t="s">
+        <v>337</v>
+      </c>
+      <c r="E227" t="s">
+        <v>306</v>
+      </c>
+      <c r="F227" t="s">
+        <v>338</v>
+      </c>
+      <c r="H227">
+        <v>200</v>
+      </c>
+      <c r="K227">
+        <v>1250000</v>
+      </c>
+      <c r="U227">
+        <v>1</v>
+      </c>
+      <c r="V227">
+        <v>70</v>
+      </c>
+      <c r="W227">
+        <v>150</v>
+      </c>
+      <c r="X227" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="228" spans="1:27">
+      <c r="A228" t="s">
+        <v>429</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+      <c r="D228" t="s">
+        <v>52</v>
+      </c>
+      <c r="E228" t="s">
+        <v>28</v>
+      </c>
+      <c r="F228" t="s">
+        <v>53</v>
+      </c>
+      <c r="H228">
+        <v>8</v>
+      </c>
+      <c r="K228">
+        <v>50</v>
+      </c>
+      <c r="O228">
+        <v>0.05</v>
+      </c>
+      <c r="P228">
+        <v>0.05</v>
+      </c>
+      <c r="Q228">
+        <v>0.05</v>
+      </c>
+      <c r="R228">
+        <v>0.05</v>
+      </c>
+      <c r="S228">
+        <v>0.05</v>
+      </c>
+      <c r="U228">
+        <v>1</v>
+      </c>
+      <c r="V228">
+        <v>3</v>
+      </c>
+      <c r="W228">
+        <v>8</v>
+      </c>
+      <c r="X228" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="229" spans="1:27">
+      <c r="B229" t="s">
+        <v>452</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229" t="s">
+        <v>240</v>
+      </c>
+      <c r="E229" t="s">
+        <v>28</v>
+      </c>
+      <c r="F229" t="s">
+        <v>241</v>
+      </c>
+      <c r="H229">
+        <v>380</v>
+      </c>
+      <c r="K229">
+        <v>750000</v>
+      </c>
+      <c r="O229">
+        <v>0.35</v>
+      </c>
+      <c r="P229">
+        <v>0.35</v>
+      </c>
+      <c r="Q229">
+        <v>0.35</v>
+      </c>
+      <c r="R229">
+        <v>0.35</v>
+      </c>
+      <c r="S229">
+        <v>0.35</v>
+      </c>
+      <c r="U229">
+        <v>1</v>
+      </c>
+      <c r="V229">
+        <v>60</v>
+      </c>
+      <c r="W229">
+        <v>130</v>
+      </c>
+      <c r="X229" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="230" spans="1:27">
+      <c r="A230" t="s">
+        <v>444</v>
+      </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+      <c r="D230" t="s">
+        <v>210</v>
+      </c>
+      <c r="E230" t="s">
+        <v>28</v>
+      </c>
+      <c r="F230" t="s">
+        <v>211</v>
+      </c>
+      <c r="H230">
+        <v>280</v>
+      </c>
+      <c r="K230">
+        <v>125000</v>
+      </c>
+      <c r="O230">
+        <v>0.29</v>
+      </c>
+      <c r="P230">
+        <v>0.29</v>
+      </c>
+      <c r="Q230">
+        <v>0.29</v>
+      </c>
+      <c r="R230">
+        <v>0.29</v>
+      </c>
+      <c r="S230">
+        <v>0.29</v>
+      </c>
+      <c r="U230">
+        <v>1</v>
+      </c>
+      <c r="V230">
+        <v>50</v>
+      </c>
+      <c r="W230">
+        <v>100</v>
+      </c>
+      <c r="X230" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="231" spans="1:27">
+      <c r="B231" t="s">
+        <v>434</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+      <c r="D231" t="s">
+        <v>102</v>
+      </c>
+      <c r="E231" t="s">
+        <v>31</v>
+      </c>
+      <c r="F231" t="s">
+        <v>103</v>
+      </c>
+      <c r="G231" t="s">
+        <v>31</v>
+      </c>
+      <c r="J231">
+        <v>40</v>
+      </c>
+      <c r="K231">
+        <v>750</v>
+      </c>
+      <c r="O231">
+        <v>0.18</v>
+      </c>
+      <c r="P231">
+        <v>0.18</v>
+      </c>
+      <c r="Q231">
+        <v>0.18</v>
+      </c>
+      <c r="R231">
+        <v>0.18</v>
+      </c>
+      <c r="S231">
+        <v>0.18</v>
+      </c>
+      <c r="U231">
+        <v>1</v>
+      </c>
+      <c r="V231">
+        <v>18</v>
+      </c>
+      <c r="W231">
+        <v>36</v>
+      </c>
+      <c r="X231" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="232" spans="1:27">
+      <c r="A232" t="s">
+        <v>444</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232" t="s">
+        <v>118</v>
+      </c>
+      <c r="E232" t="s">
+        <v>31</v>
+      </c>
+      <c r="F232" t="s">
+        <v>119</v>
+      </c>
+      <c r="G232" t="s">
+        <v>31</v>
+      </c>
+      <c r="J232">
+        <v>60</v>
+      </c>
+      <c r="K232">
+        <v>1760</v>
+      </c>
+      <c r="O232">
+        <v>0.2</v>
+      </c>
+      <c r="P232">
+        <v>0.2</v>
+      </c>
+      <c r="Q232">
+        <v>0.2</v>
+      </c>
+      <c r="R232">
+        <v>0.2</v>
+      </c>
+      <c r="S232">
+        <v>0.2</v>
+      </c>
+      <c r="U232">
+        <v>1</v>
+      </c>
+      <c r="V232">
+        <v>24</v>
+      </c>
+      <c r="W232">
+        <v>40</v>
+      </c>
+      <c r="X232" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="233" spans="1:27">
+      <c r="B233" t="s">
+        <v>447</v>
+      </c>
+      <c r="C233">
+        <v>1</v>
+      </c>
+      <c r="D233" t="s">
+        <v>98</v>
+      </c>
+      <c r="E233" t="s">
+        <v>50</v>
+      </c>
+      <c r="F233" t="s">
+        <v>99</v>
+      </c>
+      <c r="G233" t="s">
+        <v>50</v>
+      </c>
+      <c r="J233">
+        <v>10</v>
+      </c>
+      <c r="K233">
+        <v>200</v>
+      </c>
+      <c r="O233">
+        <v>0.03</v>
+      </c>
+      <c r="P233">
+        <v>0.03</v>
+      </c>
+      <c r="Q233">
+        <v>0.03</v>
+      </c>
+      <c r="R233">
+        <v>0.03</v>
+      </c>
+      <c r="S233">
+        <v>0.03</v>
+      </c>
+      <c r="U233">
+        <v>1</v>
+      </c>
+      <c r="V233">
+        <v>10</v>
+      </c>
+      <c r="W233">
+        <v>20</v>
+      </c>
+      <c r="X233" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="234" spans="1:27">
+      <c r="B234" t="s">
+        <v>446</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234" t="s">
+        <v>289</v>
+      </c>
+      <c r="E234" t="s">
+        <v>273</v>
+      </c>
+      <c r="F234" t="s">
+        <v>290</v>
+      </c>
+      <c r="H234">
+        <v>55</v>
+      </c>
+      <c r="K234">
+        <v>13400</v>
+      </c>
+      <c r="L234">
+        <v>0.16</v>
+      </c>
+      <c r="M234">
+        <v>0.16</v>
+      </c>
+      <c r="N234">
+        <v>0.16</v>
+      </c>
+      <c r="U234">
+        <v>1</v>
+      </c>
+      <c r="V234">
+        <v>36</v>
+      </c>
+      <c r="W234">
+        <v>70</v>
+      </c>
+      <c r="X234" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="235" spans="1:27">
+      <c r="A235" t="s">
+        <v>448</v>
+      </c>
+      <c r="C235">
+        <v>1</v>
+      </c>
+      <c r="D235" t="s">
+        <v>102</v>
+      </c>
+      <c r="E235" t="s">
+        <v>31</v>
+      </c>
+      <c r="F235" t="s">
+        <v>103</v>
+      </c>
+      <c r="G235" t="s">
+        <v>31</v>
+      </c>
+      <c r="J235">
+        <v>40</v>
+      </c>
+      <c r="K235">
+        <v>750</v>
+      </c>
+      <c r="O235">
+        <v>0.18</v>
+      </c>
+      <c r="P235">
+        <v>0.18</v>
+      </c>
+      <c r="Q235">
+        <v>0.18</v>
+      </c>
+      <c r="R235">
+        <v>0.18</v>
+      </c>
+      <c r="S235">
+        <v>0.18</v>
+      </c>
+      <c r="U235">
+        <v>1</v>
+      </c>
+      <c r="V235">
+        <v>18</v>
+      </c>
+      <c r="W235">
+        <v>36</v>
+      </c>
+      <c r="X235" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="236" spans="1:27">
+      <c r="B236" t="s">
+        <v>438</v>
+      </c>
+      <c r="C236">
+        <v>1</v>
+      </c>
+      <c r="D236" t="s">
+        <v>102</v>
+      </c>
+      <c r="E236" t="s">
+        <v>31</v>
+      </c>
+      <c r="F236" t="s">
+        <v>103</v>
+      </c>
+      <c r="G236" t="s">
+        <v>31</v>
+      </c>
+      <c r="J236">
+        <v>40</v>
+      </c>
+      <c r="K236">
+        <v>750</v>
+      </c>
+      <c r="O236">
+        <v>0.18</v>
+      </c>
+      <c r="P236">
+        <v>0.18</v>
+      </c>
+      <c r="Q236">
+        <v>0.18</v>
+      </c>
+      <c r="R236">
+        <v>0.18</v>
+      </c>
+      <c r="S236">
+        <v>0.18</v>
+      </c>
+      <c r="U236">
+        <v>1</v>
+      </c>
+      <c r="V236">
+        <v>18</v>
+      </c>
+      <c r="W236">
+        <v>36</v>
+      </c>
+      <c r="X236" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="237" spans="1:27">
+      <c r="A237" t="s">
+        <v>440</v>
+      </c>
+      <c r="C237">
+        <v>1</v>
+      </c>
+      <c r="D237" t="s">
+        <v>228</v>
+      </c>
+      <c r="E237" t="s">
+        <v>31</v>
+      </c>
+      <c r="F237" t="s">
+        <v>229</v>
+      </c>
+      <c r="G237" t="s">
+        <v>31</v>
+      </c>
+      <c r="J237">
+        <v>230</v>
+      </c>
+      <c r="K237">
+        <v>450000</v>
+      </c>
+      <c r="O237">
+        <v>0.4</v>
+      </c>
+      <c r="P237">
+        <v>0.4</v>
+      </c>
+      <c r="Q237">
+        <v>0.4</v>
+      </c>
+      <c r="R237">
+        <v>0.4</v>
+      </c>
+      <c r="S237">
+        <v>0.4</v>
+      </c>
+      <c r="U237">
+        <v>1</v>
+      </c>
+      <c r="V237">
+        <v>55</v>
+      </c>
+      <c r="W237">
+        <v>110</v>
+      </c>
+      <c r="X237" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="238" spans="1:27">
+      <c r="A238" t="s">
+        <v>453</v>
+      </c>
+      <c r="C238">
+        <v>1</v>
+      </c>
+      <c r="D238" t="s">
+        <v>118</v>
+      </c>
+      <c r="E238" t="s">
+        <v>31</v>
+      </c>
+      <c r="F238" t="s">
+        <v>119</v>
+      </c>
+      <c r="G238" t="s">
+        <v>31</v>
+      </c>
+      <c r="J238">
+        <v>60</v>
+      </c>
+      <c r="K238">
+        <v>1760</v>
+      </c>
+      <c r="O238">
+        <v>0.2</v>
+      </c>
+      <c r="P238">
+        <v>0.2</v>
+      </c>
+      <c r="Q238">
+        <v>0.2</v>
+      </c>
+      <c r="R238">
+        <v>0.2</v>
+      </c>
+      <c r="S238">
+        <v>0.2</v>
+      </c>
+      <c r="U238">
+        <v>1</v>
+      </c>
+      <c r="V238">
+        <v>24</v>
+      </c>
+      <c r="W238">
+        <v>40</v>
+      </c>
+      <c r="X238" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="239" spans="1:27">
+      <c r="A239" t="s">
+        <v>436</v>
+      </c>
+      <c r="C239">
+        <v>1</v>
+      </c>
+      <c r="D239" t="s">
+        <v>327</v>
+      </c>
+      <c r="E239" t="s">
+        <v>306</v>
+      </c>
+      <c r="F239" t="s">
+        <v>328</v>
+      </c>
+      <c r="H239">
+        <v>120</v>
+      </c>
+      <c r="K239">
+        <v>55000</v>
+      </c>
+      <c r="U239">
+        <v>1</v>
+      </c>
+      <c r="V239">
+        <v>43</v>
+      </c>
+      <c r="W239">
+        <v>78</v>
+      </c>
+      <c r="X239" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="240" spans="1:27">
+      <c r="A240" t="s">
+        <v>440</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240" t="s">
+        <v>301</v>
+      </c>
+      <c r="E240" t="s">
+        <v>273</v>
+      </c>
+      <c r="F240" t="s">
+        <v>302</v>
+      </c>
+      <c r="H240">
+        <v>90</v>
+      </c>
+      <c r="K240">
+        <v>750000</v>
+      </c>
+      <c r="L240">
+        <v>0.29</v>
+      </c>
+      <c r="M240">
+        <v>0.29</v>
+      </c>
+      <c r="N240">
+        <v>0.29</v>
+      </c>
+      <c r="U240">
+        <v>1</v>
+      </c>
+      <c r="V240">
+        <v>60</v>
+      </c>
+      <c r="W240">
+        <v>130</v>
+      </c>
+      <c r="X240" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="241" spans="1:27">
+      <c r="A241" t="s">
+        <v>429</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+      <c r="D241" t="s">
+        <v>270</v>
+      </c>
+      <c r="E241" t="s">
+        <v>50</v>
+      </c>
+      <c r="F241" t="s">
+        <v>271</v>
+      </c>
+      <c r="G241" t="s">
+        <v>50</v>
+      </c>
+      <c r="J241">
+        <v>200</v>
+      </c>
+      <c r="K241">
+        <v>800000</v>
+      </c>
+      <c r="O241">
+        <v>0.23</v>
+      </c>
+      <c r="P241">
+        <v>0.23</v>
+      </c>
+      <c r="Q241">
+        <v>0.23</v>
+      </c>
+      <c r="R241">
+        <v>0.23</v>
+      </c>
+      <c r="S241">
+        <v>0.23</v>
+      </c>
+      <c r="U241">
+        <v>1</v>
+      </c>
+      <c r="V241">
+        <v>70</v>
+      </c>
+      <c r="W241">
+        <v>180</v>
+      </c>
+      <c r="X241" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="242" spans="1:27">
+      <c r="A242" t="s">
+        <v>429</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="D242" t="s">
+        <v>299</v>
+      </c>
+      <c r="E242" t="s">
+        <v>273</v>
+      </c>
+      <c r="F242" t="s">
+        <v>300</v>
+      </c>
+      <c r="H242">
+        <v>80</v>
+      </c>
+      <c r="K242">
+        <v>346000</v>
+      </c>
+      <c r="L242">
+        <v>0.27</v>
+      </c>
+      <c r="M242">
+        <v>0.27</v>
+      </c>
+      <c r="N242">
+        <v>0.27</v>
+      </c>
+      <c r="U242">
+        <v>1</v>
+      </c>
+      <c r="V242">
+        <v>55</v>
+      </c>
+      <c r="W242">
+        <v>110</v>
+      </c>
+      <c r="X242" t="s">
         <v>273</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated items data dump
</commit_message>
<xml_diff>
--- a/resources/data-imports/items.xlsx
+++ b/resources/data-imports/items.xlsx
@@ -1715,7 +1715,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA242"/>
+  <dimension ref="A1:AA247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -5025,6 +5025,9 @@
       <c r="F77" t="s">
         <v>187</v>
       </c>
+      <c r="G77" t="s">
+        <v>38</v>
+      </c>
       <c r="J77">
         <v>90</v>
       </c>
@@ -11582,6 +11585,223 @@
       </c>
       <c r="X242" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="243" spans="1:27">
+      <c r="B243" t="s">
+        <v>432</v>
+      </c>
+      <c r="C243">
+        <v>1</v>
+      </c>
+      <c r="D243" t="s">
+        <v>132</v>
+      </c>
+      <c r="E243" t="s">
+        <v>28</v>
+      </c>
+      <c r="F243" t="s">
+        <v>133</v>
+      </c>
+      <c r="H243">
+        <v>145</v>
+      </c>
+      <c r="K243">
+        <v>3600</v>
+      </c>
+      <c r="O243">
+        <v>0.2</v>
+      </c>
+      <c r="P243">
+        <v>0.2</v>
+      </c>
+      <c r="Q243">
+        <v>0.2</v>
+      </c>
+      <c r="R243">
+        <v>0.2</v>
+      </c>
+      <c r="S243">
+        <v>0.2</v>
+      </c>
+      <c r="U243">
+        <v>1</v>
+      </c>
+      <c r="V243">
+        <v>28</v>
+      </c>
+      <c r="W243">
+        <v>50</v>
+      </c>
+      <c r="X243" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="244" spans="1:27">
+      <c r="A244" t="s">
+        <v>443</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+      <c r="D244" t="s">
+        <v>30</v>
+      </c>
+      <c r="E244" t="s">
+        <v>31</v>
+      </c>
+      <c r="F244" t="s">
+        <v>32</v>
+      </c>
+      <c r="G244" t="s">
+        <v>31</v>
+      </c>
+      <c r="J244">
+        <v>4</v>
+      </c>
+      <c r="K244">
+        <v>10</v>
+      </c>
+      <c r="U244">
+        <v>1</v>
+      </c>
+      <c r="V244">
+        <v>1</v>
+      </c>
+      <c r="W244">
+        <v>5</v>
+      </c>
+      <c r="X244" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="245" spans="1:27">
+      <c r="B245" t="s">
+        <v>439</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245" t="s">
+        <v>64</v>
+      </c>
+      <c r="E245" t="s">
+        <v>47</v>
+      </c>
+      <c r="F245" t="s">
+        <v>65</v>
+      </c>
+      <c r="G245" t="s">
+        <v>47</v>
+      </c>
+      <c r="J245">
+        <v>3</v>
+      </c>
+      <c r="K245">
+        <v>55</v>
+      </c>
+      <c r="U245">
+        <v>1</v>
+      </c>
+      <c r="V245">
+        <v>3</v>
+      </c>
+      <c r="W245">
+        <v>8</v>
+      </c>
+      <c r="X245" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="246" spans="1:27">
+      <c r="A246" t="s">
+        <v>451</v>
+      </c>
+      <c r="C246">
+        <v>1</v>
+      </c>
+      <c r="D246" t="s">
+        <v>186</v>
+      </c>
+      <c r="E246" t="s">
+        <v>38</v>
+      </c>
+      <c r="F246" t="s">
+        <v>187</v>
+      </c>
+      <c r="G246" t="s">
+        <v>38</v>
+      </c>
+      <c r="J246">
+        <v>90</v>
+      </c>
+      <c r="K246">
+        <v>18000</v>
+      </c>
+      <c r="O246">
+        <v>0.14</v>
+      </c>
+      <c r="P246">
+        <v>0.14</v>
+      </c>
+      <c r="Q246">
+        <v>0.14</v>
+      </c>
+      <c r="R246">
+        <v>0.14</v>
+      </c>
+      <c r="S246">
+        <v>0.14</v>
+      </c>
+      <c r="U246">
+        <v>1</v>
+      </c>
+      <c r="V246">
+        <v>40</v>
+      </c>
+      <c r="W246">
+        <v>75</v>
+      </c>
+      <c r="X246" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="247" spans="1:27">
+      <c r="A247" t="s">
+        <v>435</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+      <c r="D247" t="s">
+        <v>74</v>
+      </c>
+      <c r="E247" t="s">
+        <v>38</v>
+      </c>
+      <c r="F247" t="s">
+        <v>75</v>
+      </c>
+      <c r="G247" t="s">
+        <v>38</v>
+      </c>
+      <c r="J247">
+        <v>5</v>
+      </c>
+      <c r="K247">
+        <v>100</v>
+      </c>
+      <c r="U247">
+        <v>1</v>
+      </c>
+      <c r="V247">
+        <v>6</v>
+      </c>
+      <c r="W247">
+        <v>12</v>
+      </c>
+      <c r="X247" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data items with more alchemy items.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items.xlsx
+++ b/resources/data-imports/items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/1.1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433EBCA3-1191-D64D-A5E0-4137B94A5E2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25420747-DE27-2249-9324-6A8D75C7972A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2990" uniqueCount="1311">
   <si>
     <t>item_suffix_id</t>
   </si>
@@ -3940,6 +3940,30 @@
   </si>
   <si>
     <t>Demonic Bomb</t>
+  </si>
+  <si>
+    <t>Demonic Blood</t>
+  </si>
+  <si>
+    <t>Alchemists Eye</t>
+  </si>
+  <si>
+    <t>Astral Mages Ink</t>
+  </si>
+  <si>
+    <t>Enhancement Dust</t>
+  </si>
+  <si>
+    <t>Crafters Crystal Ball</t>
+  </si>
+  <si>
+    <t>Postion of Inspiration</t>
+  </si>
+  <si>
+    <t>Disenchantment Candle</t>
+  </si>
+  <si>
+    <t>Deaths Cloud</t>
   </si>
 </sst>
 </file>
@@ -4279,10 +4303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY637"/>
+  <dimension ref="A1:AY645"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
-      <selection activeCell="A599" sqref="A599:XFD599"/>
+    <sheetView tabSelected="1" topLeftCell="A597" workbookViewId="0">
+      <selection activeCell="AJ650" sqref="AJ650"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53050,7 +53074,7 @@
         <v>15</v>
       </c>
       <c r="AB637">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="AC637" t="s">
         <v>1276</v>
@@ -53098,6 +53122,667 @@
         <v>0</v>
       </c>
       <c r="AY637">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C638">
+        <v>1</v>
+      </c>
+      <c r="D638" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E638" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F638" t="s">
+        <v>1292</v>
+      </c>
+      <c r="K638">
+        <v>0</v>
+      </c>
+      <c r="L638">
+        <v>5000</v>
+      </c>
+      <c r="M638">
+        <v>40</v>
+      </c>
+      <c r="Y638">
+        <v>1</v>
+      </c>
+      <c r="AA638">
+        <v>20</v>
+      </c>
+      <c r="AB638">
+        <v>40</v>
+      </c>
+      <c r="AC638" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF638">
+        <v>0</v>
+      </c>
+      <c r="AG638">
+        <v>0</v>
+      </c>
+      <c r="AH638">
+        <v>0</v>
+      </c>
+      <c r="AI638">
+        <v>0</v>
+      </c>
+      <c r="AJ638">
+        <v>0</v>
+      </c>
+      <c r="AL638">
+        <v>1</v>
+      </c>
+      <c r="AM638">
+        <v>1</v>
+      </c>
+      <c r="AO638">
+        <v>0</v>
+      </c>
+      <c r="AP638">
+        <v>20</v>
+      </c>
+      <c r="AQ638">
+        <v>1</v>
+      </c>
+      <c r="AR638">
+        <v>0.05</v>
+      </c>
+      <c r="AT638">
+        <v>0</v>
+      </c>
+      <c r="AU638">
+        <v>0</v>
+      </c>
+      <c r="AW638">
+        <v>0</v>
+      </c>
+      <c r="AX638">
+        <v>0</v>
+      </c>
+      <c r="AY638">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C639">
+        <v>1</v>
+      </c>
+      <c r="D639" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E639" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F639" t="s">
+        <v>1295</v>
+      </c>
+      <c r="K639">
+        <v>0</v>
+      </c>
+      <c r="L639">
+        <v>10000</v>
+      </c>
+      <c r="M639">
+        <v>60</v>
+      </c>
+      <c r="Y639">
+        <v>1</v>
+      </c>
+      <c r="AA639">
+        <v>25</v>
+      </c>
+      <c r="AB639">
+        <v>40</v>
+      </c>
+      <c r="AC639" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF639">
+        <v>0</v>
+      </c>
+      <c r="AG639">
+        <v>0</v>
+      </c>
+      <c r="AH639">
+        <v>0</v>
+      </c>
+      <c r="AI639">
+        <v>0</v>
+      </c>
+      <c r="AJ639">
+        <v>0</v>
+      </c>
+      <c r="AL639">
+        <v>1</v>
+      </c>
+      <c r="AM639">
+        <v>1</v>
+      </c>
+      <c r="AO639">
+        <v>0</v>
+      </c>
+      <c r="AP639">
+        <v>20</v>
+      </c>
+      <c r="AR639">
+        <v>0</v>
+      </c>
+      <c r="AS639">
+        <v>4</v>
+      </c>
+      <c r="AT639">
+        <v>0.1</v>
+      </c>
+      <c r="AU639">
+        <v>0.01</v>
+      </c>
+      <c r="AW639">
+        <v>0</v>
+      </c>
+      <c r="AX639">
+        <v>0</v>
+      </c>
+      <c r="AY639">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C640">
+        <v>1</v>
+      </c>
+      <c r="D640" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E640" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F640" t="s">
+        <v>1280</v>
+      </c>
+      <c r="K640">
+        <v>0</v>
+      </c>
+      <c r="L640">
+        <v>10000</v>
+      </c>
+      <c r="M640">
+        <v>60</v>
+      </c>
+      <c r="Y640">
+        <v>1</v>
+      </c>
+      <c r="AA640">
+        <v>25</v>
+      </c>
+      <c r="AB640">
+        <v>40</v>
+      </c>
+      <c r="AC640" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF640">
+        <v>0</v>
+      </c>
+      <c r="AG640">
+        <v>0</v>
+      </c>
+      <c r="AH640">
+        <v>0</v>
+      </c>
+      <c r="AI640">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AJ640">
+        <v>0</v>
+      </c>
+      <c r="AL640">
+        <v>1</v>
+      </c>
+      <c r="AM640">
+        <v>1</v>
+      </c>
+      <c r="AO640">
+        <v>0</v>
+      </c>
+      <c r="AP640">
+        <v>20</v>
+      </c>
+      <c r="AR640">
+        <v>0</v>
+      </c>
+      <c r="AS640">
+        <v>5</v>
+      </c>
+      <c r="AT640">
+        <v>0</v>
+      </c>
+      <c r="AU640">
+        <v>0.01</v>
+      </c>
+      <c r="AW640">
+        <v>0</v>
+      </c>
+      <c r="AX640">
+        <v>0</v>
+      </c>
+      <c r="AY640">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C641">
+        <v>1</v>
+      </c>
+      <c r="D641" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E641" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F641" t="s">
+        <v>1298</v>
+      </c>
+      <c r="K641">
+        <v>0</v>
+      </c>
+      <c r="L641">
+        <v>10000</v>
+      </c>
+      <c r="M641">
+        <v>60</v>
+      </c>
+      <c r="Y641">
+        <v>1</v>
+      </c>
+      <c r="AA641">
+        <v>25</v>
+      </c>
+      <c r="AB641">
+        <v>40</v>
+      </c>
+      <c r="AC641" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF641">
+        <v>0</v>
+      </c>
+      <c r="AG641">
+        <v>0</v>
+      </c>
+      <c r="AH641">
+        <v>0</v>
+      </c>
+      <c r="AI641">
+        <v>0</v>
+      </c>
+      <c r="AJ641">
+        <v>0</v>
+      </c>
+      <c r="AL641">
+        <v>1</v>
+      </c>
+      <c r="AM641">
+        <v>1</v>
+      </c>
+      <c r="AO641">
+        <v>0</v>
+      </c>
+      <c r="AP641">
+        <v>20</v>
+      </c>
+      <c r="AR641">
+        <v>0</v>
+      </c>
+      <c r="AS641">
+        <v>0</v>
+      </c>
+      <c r="AT641">
+        <v>0.01</v>
+      </c>
+      <c r="AU641">
+        <v>0.01</v>
+      </c>
+      <c r="AW641">
+        <v>0</v>
+      </c>
+      <c r="AX641">
+        <v>0</v>
+      </c>
+      <c r="AY641">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C642">
+        <v>1</v>
+      </c>
+      <c r="D642" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E642" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F642" t="s">
+        <v>1284</v>
+      </c>
+      <c r="K642">
+        <v>0</v>
+      </c>
+      <c r="L642">
+        <v>10000</v>
+      </c>
+      <c r="M642">
+        <v>60</v>
+      </c>
+      <c r="Y642">
+        <v>1</v>
+      </c>
+      <c r="AA642">
+        <v>25</v>
+      </c>
+      <c r="AB642">
+        <v>40</v>
+      </c>
+      <c r="AC642" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF642">
+        <v>0</v>
+      </c>
+      <c r="AG642">
+        <v>0</v>
+      </c>
+      <c r="AH642">
+        <v>0</v>
+      </c>
+      <c r="AI642">
+        <v>0</v>
+      </c>
+      <c r="AJ642">
+        <v>0</v>
+      </c>
+      <c r="AL642">
+        <v>1</v>
+      </c>
+      <c r="AM642">
+        <v>1</v>
+      </c>
+      <c r="AO642">
+        <v>0</v>
+      </c>
+      <c r="AP642">
+        <v>20</v>
+      </c>
+      <c r="AR642">
+        <v>0</v>
+      </c>
+      <c r="AS642">
+        <v>1</v>
+      </c>
+      <c r="AT642">
+        <v>0.01</v>
+      </c>
+      <c r="AU642">
+        <v>0.01</v>
+      </c>
+      <c r="AW642">
+        <v>0</v>
+      </c>
+      <c r="AX642">
+        <v>0</v>
+      </c>
+      <c r="AY642">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="643" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C643">
+        <v>1</v>
+      </c>
+      <c r="D643" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E643" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F643" t="s">
+        <v>1286</v>
+      </c>
+      <c r="K643">
+        <v>0</v>
+      </c>
+      <c r="L643">
+        <v>10000</v>
+      </c>
+      <c r="M643">
+        <v>60</v>
+      </c>
+      <c r="Y643">
+        <v>1</v>
+      </c>
+      <c r="AA643">
+        <v>25</v>
+      </c>
+      <c r="AB643">
+        <v>40</v>
+      </c>
+      <c r="AC643" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF643">
+        <v>0</v>
+      </c>
+      <c r="AG643">
+        <v>0</v>
+      </c>
+      <c r="AH643">
+        <v>0</v>
+      </c>
+      <c r="AI643">
+        <v>0</v>
+      </c>
+      <c r="AJ643">
+        <v>0</v>
+      </c>
+      <c r="AL643">
+        <v>1</v>
+      </c>
+      <c r="AM643">
+        <v>1</v>
+      </c>
+      <c r="AO643">
+        <v>0</v>
+      </c>
+      <c r="AP643">
+        <v>20</v>
+      </c>
+      <c r="AR643">
+        <v>0</v>
+      </c>
+      <c r="AS643">
+        <v>2</v>
+      </c>
+      <c r="AT643">
+        <v>0.01</v>
+      </c>
+      <c r="AU643">
+        <v>0.01</v>
+      </c>
+      <c r="AW643">
+        <v>0</v>
+      </c>
+      <c r="AX643">
+        <v>0</v>
+      </c>
+      <c r="AY643">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="644" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C644">
+        <v>1</v>
+      </c>
+      <c r="D644" t="s">
+        <v>1309</v>
+      </c>
+      <c r="E644" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F644" t="s">
+        <v>1288</v>
+      </c>
+      <c r="K644">
+        <v>0</v>
+      </c>
+      <c r="L644">
+        <v>10000</v>
+      </c>
+      <c r="M644">
+        <v>60</v>
+      </c>
+      <c r="Y644">
+        <v>1</v>
+      </c>
+      <c r="AA644">
+        <v>25</v>
+      </c>
+      <c r="AB644">
+        <v>40</v>
+      </c>
+      <c r="AC644" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF644">
+        <v>0</v>
+      </c>
+      <c r="AG644">
+        <v>0</v>
+      </c>
+      <c r="AH644">
+        <v>0</v>
+      </c>
+      <c r="AI644">
+        <v>0</v>
+      </c>
+      <c r="AJ644">
+        <v>0</v>
+      </c>
+      <c r="AL644">
+        <v>1</v>
+      </c>
+      <c r="AM644">
+        <v>1</v>
+      </c>
+      <c r="AO644">
+        <v>0</v>
+      </c>
+      <c r="AP644">
+        <v>20</v>
+      </c>
+      <c r="AR644">
+        <v>0</v>
+      </c>
+      <c r="AS644">
+        <v>3</v>
+      </c>
+      <c r="AT644">
+        <v>0.01</v>
+      </c>
+      <c r="AU644">
+        <v>0.01</v>
+      </c>
+      <c r="AW644">
+        <v>0</v>
+      </c>
+      <c r="AX644">
+        <v>0</v>
+      </c>
+      <c r="AY644">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="645" spans="3:51" x14ac:dyDescent="0.2">
+      <c r="C645">
+        <v>1</v>
+      </c>
+      <c r="D645" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E645" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F645" t="s">
+        <v>1290</v>
+      </c>
+      <c r="K645">
+        <v>0</v>
+      </c>
+      <c r="L645">
+        <v>30000</v>
+      </c>
+      <c r="M645">
+        <v>100</v>
+      </c>
+      <c r="Y645">
+        <v>1</v>
+      </c>
+      <c r="AA645">
+        <v>30</v>
+      </c>
+      <c r="AB645">
+        <v>60</v>
+      </c>
+      <c r="AC645" t="s">
+        <v>1276</v>
+      </c>
+      <c r="AF645">
+        <v>0</v>
+      </c>
+      <c r="AG645">
+        <v>0</v>
+      </c>
+      <c r="AH645">
+        <v>0</v>
+      </c>
+      <c r="AI645">
+        <v>0</v>
+      </c>
+      <c r="AJ645">
+        <v>0</v>
+      </c>
+      <c r="AL645">
+        <v>1</v>
+      </c>
+      <c r="AM645">
+        <v>1</v>
+      </c>
+      <c r="AN645">
+        <v>1</v>
+      </c>
+      <c r="AO645">
+        <v>0.1</v>
+      </c>
+      <c r="AR645">
+        <v>0</v>
+      </c>
+      <c r="AT645">
+        <v>0</v>
+      </c>
+      <c r="AU645">
+        <v>0</v>
+      </c>
+      <c r="AW645">
+        <v>0</v>
+      </c>
+      <c r="AX645">
+        <v>0</v>
+      </c>
+      <c r="AY645">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated monsters to heal and use affixes.
- Updated monster show page.
- Updated monster model, table and transformer.
- Updated data imports.
- We are ready to make the monster attack now (with everything it has).
</commit_message>
<xml_diff>
--- a/resources/data-imports/items.xlsx
+++ b/resources/data-imports/items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1333">
   <si>
     <t>item_suffix_id</t>
   </si>
@@ -3951,6 +3951,30 @@
   </si>
   <si>
     <t>Deaths Cloud</t>
+  </si>
+  <si>
+    <t>Quick Feet</t>
+  </si>
+  <si>
+    <t>Move across the land quickly child. The creatures are chasing you.</t>
+  </si>
+  <si>
+    <t>Shattered Shards</t>
+  </si>
+  <si>
+    <t>With this, all your training skills will increase by a % for a specific amount of time.</t>
+  </si>
+  <si>
+    <t>Golden Illusions</t>
+  </si>
+  <si>
+    <t>Create illusions out of gold dust child. These can make you seem stronger and more attuned then you might be.</t>
+  </si>
+  <si>
+    <t>Broken Mirror</t>
+  </si>
+  <si>
+    <t>Look into this broken mirror child. Do you see it? Do you feel it? The strength you need to survive.</t>
   </si>
   <si>
     <t>Bland Potion</t>
@@ -4328,7 +4352,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AY629"/>
+  <dimension ref="A1:AY633"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -5144,9 +5168,6 @@
       <c r="Y9">
         <v>1</v>
       </c>
-      <c r="Z9">
-        <v>1</v>
-      </c>
       <c r="AA9">
         <v>30</v>
       </c>
@@ -8086,9 +8107,6 @@
       <c r="Y46">
         <v>1</v>
       </c>
-      <c r="Z46">
-        <v>1</v>
-      </c>
       <c r="AA46">
         <v>30</v>
       </c>
@@ -10820,9 +10838,6 @@
       <c r="Y84">
         <v>1</v>
       </c>
-      <c r="Z84">
-        <v>1</v>
-      </c>
       <c r="AA84">
         <v>30</v>
       </c>
@@ -13475,9 +13490,6 @@
       <c r="Y120">
         <v>1</v>
       </c>
-      <c r="Z120">
-        <v>1</v>
-      </c>
       <c r="AA120">
         <v>28</v>
       </c>
@@ -14167,19 +14179,19 @@
         <v>30000</v>
       </c>
       <c r="Q128">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="R128">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="S128">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="T128">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="U128">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="V128">
         <v>0.35</v>
@@ -16853,9 +16865,6 @@
       <c r="Y159">
         <v>1</v>
       </c>
-      <c r="Z159">
-        <v>1</v>
-      </c>
       <c r="AA159">
         <v>28</v>
       </c>
@@ -19459,9 +19468,6 @@
       <c r="Y196">
         <v>1</v>
       </c>
-      <c r="Z196">
-        <v>1</v>
-      </c>
       <c r="AA196">
         <v>30</v>
       </c>
@@ -22571,8 +22577,44 @@
       <c r="AE240">
         <v>0.45</v>
       </c>
+      <c r="AF240">
+        <v>0</v>
+      </c>
+      <c r="AG240">
+        <v>0</v>
+      </c>
+      <c r="AH240">
+        <v>0</v>
+      </c>
+      <c r="AI240">
+        <v>0</v>
+      </c>
+      <c r="AJ240">
+        <v>0</v>
+      </c>
       <c r="AK240">
         <v>0.45</v>
+      </c>
+      <c r="AO240">
+        <v>0</v>
+      </c>
+      <c r="AR240">
+        <v>0</v>
+      </c>
+      <c r="AT240">
+        <v>0</v>
+      </c>
+      <c r="AU240">
+        <v>0</v>
+      </c>
+      <c r="AW240">
+        <v>0</v>
+      </c>
+      <c r="AX240">
+        <v>0</v>
+      </c>
+      <c r="AY240">
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:51">
@@ -22603,8 +22645,44 @@
       <c r="AE241">
         <v>0.45</v>
       </c>
+      <c r="AF241">
+        <v>0</v>
+      </c>
+      <c r="AG241">
+        <v>0</v>
+      </c>
+      <c r="AH241">
+        <v>0</v>
+      </c>
+      <c r="AI241">
+        <v>0</v>
+      </c>
+      <c r="AJ241">
+        <v>0</v>
+      </c>
       <c r="AK241">
         <v>0.45</v>
+      </c>
+      <c r="AO241">
+        <v>0</v>
+      </c>
+      <c r="AR241">
+        <v>0</v>
+      </c>
+      <c r="AT241">
+        <v>0</v>
+      </c>
+      <c r="AU241">
+        <v>0</v>
+      </c>
+      <c r="AW241">
+        <v>0</v>
+      </c>
+      <c r="AX241">
+        <v>0</v>
+      </c>
+      <c r="AY241">
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:51">
@@ -22632,6 +22710,42 @@
       <c r="X242" t="s">
         <v>551</v>
       </c>
+      <c r="AF242">
+        <v>0</v>
+      </c>
+      <c r="AG242">
+        <v>0</v>
+      </c>
+      <c r="AH242">
+        <v>0</v>
+      </c>
+      <c r="AI242">
+        <v>0</v>
+      </c>
+      <c r="AJ242">
+        <v>0</v>
+      </c>
+      <c r="AO242">
+        <v>0</v>
+      </c>
+      <c r="AR242">
+        <v>0</v>
+      </c>
+      <c r="AT242">
+        <v>0</v>
+      </c>
+      <c r="AU242">
+        <v>0</v>
+      </c>
+      <c r="AW242">
+        <v>0</v>
+      </c>
+      <c r="AX242">
+        <v>0</v>
+      </c>
+      <c r="AY242">
+        <v>0</v>
+      </c>
     </row>
     <row r="243" spans="1:51">
       <c r="D243" t="s">
@@ -23706,9 +23820,6 @@
       <c r="Y257">
         <v>1</v>
       </c>
-      <c r="Z257">
-        <v>1</v>
-      </c>
       <c r="AA257">
         <v>28</v>
       </c>
@@ -27062,9 +27173,6 @@
       <c r="Y294">
         <v>1</v>
       </c>
-      <c r="Z294">
-        <v>1</v>
-      </c>
       <c r="AA294">
         <v>28</v>
       </c>
@@ -30418,9 +30526,6 @@
       <c r="Y331">
         <v>1</v>
       </c>
-      <c r="Z331">
-        <v>1</v>
-      </c>
       <c r="AA331">
         <v>28</v>
       </c>
@@ -31911,19 +32016,19 @@
         <v>35930000</v>
       </c>
       <c r="Q348">
-        <v>0.62</v>
+        <v>0.49</v>
       </c>
       <c r="R348">
-        <v>0.62</v>
+        <v>0.49</v>
       </c>
       <c r="S348">
-        <v>0.62</v>
+        <v>0.49</v>
       </c>
       <c r="T348">
-        <v>0.62</v>
+        <v>0.49</v>
       </c>
       <c r="U348">
-        <v>0.62</v>
+        <v>0.49</v>
       </c>
       <c r="V348">
         <v>0.62</v>
@@ -33854,9 +33959,6 @@
       <c r="Y369">
         <v>1</v>
       </c>
-      <c r="Z369">
-        <v>1</v>
-      </c>
       <c r="AA369">
         <v>28</v>
       </c>
@@ -37138,9 +37240,6 @@
       <c r="Y406">
         <v>1</v>
       </c>
-      <c r="Z406">
-        <v>1</v>
-      </c>
       <c r="AA406">
         <v>30</v>
       </c>
@@ -40056,9 +40155,6 @@
       <c r="Y443">
         <v>1</v>
       </c>
-      <c r="Z443">
-        <v>1</v>
-      </c>
       <c r="AA443">
         <v>28</v>
       </c>
@@ -43322,9 +43418,6 @@
       <c r="Y480">
         <v>1</v>
       </c>
-      <c r="Z480">
-        <v>1</v>
-      </c>
       <c r="AA480">
         <v>3</v>
       </c>
@@ -43399,9 +43492,6 @@
       <c r="Y481">
         <v>1</v>
       </c>
-      <c r="Z481">
-        <v>1</v>
-      </c>
       <c r="AA481">
         <v>3</v>
       </c>
@@ -43470,9 +43560,6 @@
       <c r="Y482">
         <v>1</v>
       </c>
-      <c r="Z482">
-        <v>1</v>
-      </c>
       <c r="AA482">
         <v>3</v>
       </c>
@@ -43541,9 +43628,6 @@
       <c r="Y483">
         <v>1</v>
       </c>
-      <c r="Z483">
-        <v>1</v>
-      </c>
       <c r="AA483">
         <v>3</v>
       </c>
@@ -43612,9 +43696,6 @@
       <c r="Y484">
         <v>1</v>
       </c>
-      <c r="Z484">
-        <v>1</v>
-      </c>
       <c r="AA484">
         <v>3</v>
       </c>
@@ -43683,9 +43764,6 @@
       <c r="Y485">
         <v>1</v>
       </c>
-      <c r="Z485">
-        <v>1</v>
-      </c>
       <c r="AA485">
         <v>3</v>
       </c>
@@ -43754,9 +43832,6 @@
       <c r="Y486">
         <v>1</v>
       </c>
-      <c r="Z486">
-        <v>1</v>
-      </c>
       <c r="AA486">
         <v>3</v>
       </c>
@@ -53899,40 +53974,31 @@
         <v>0</v>
       </c>
       <c r="L620">
-        <v>200</v>
+        <v>3500</v>
       </c>
       <c r="M620">
-        <v>8</v>
+        <v>120</v>
+      </c>
+      <c r="V620">
+        <v>0</v>
+      </c>
+      <c r="W620">
+        <v>0</v>
       </c>
       <c r="Y620">
         <v>1</v>
       </c>
-      <c r="Z620">
-        <v>1</v>
-      </c>
       <c r="AA620">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="AB620">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="AC620" t="s">
         <v>1290</v>
       </c>
-      <c r="AF620">
-        <v>0</v>
-      </c>
-      <c r="AG620">
-        <v>0</v>
-      </c>
-      <c r="AH620">
-        <v>0</v>
-      </c>
-      <c r="AI620">
-        <v>0</v>
-      </c>
       <c r="AJ620">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AL620">
         <v>1</v>
@@ -53940,31 +54006,16 @@
       <c r="AM620">
         <v>1</v>
       </c>
-      <c r="AO620">
-        <v>0</v>
-      </c>
       <c r="AP620">
-        <v>10</v>
-      </c>
-      <c r="AQ620">
-        <v>1</v>
-      </c>
-      <c r="AR620">
-        <v>0.008</v>
+        <v>22</v>
+      </c>
+      <c r="AS620">
+        <v>6</v>
       </c>
       <c r="AT620">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AU620">
-        <v>0</v>
-      </c>
-      <c r="AW620">
-        <v>0</v>
-      </c>
-      <c r="AX620">
-        <v>0</v>
-      </c>
-      <c r="AY620">
         <v>0</v>
       </c>
     </row>
@@ -53985,40 +54036,43 @@
         <v>0</v>
       </c>
       <c r="L621">
-        <v>500</v>
+        <v>4000</v>
       </c>
       <c r="M621">
-        <v>12</v>
+        <v>150</v>
+      </c>
+      <c r="V621">
+        <v>0</v>
+      </c>
+      <c r="W621">
+        <v>0</v>
       </c>
       <c r="Y621">
         <v>1</v>
       </c>
-      <c r="Z621">
-        <v>1</v>
-      </c>
       <c r="AA621">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="AB621">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="AC621" t="s">
         <v>1290</v>
       </c>
       <c r="AF621">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AG621">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AH621">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AI621">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AJ621">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AL621">
         <v>1</v>
@@ -54026,32 +54080,17 @@
       <c r="AM621">
         <v>1</v>
       </c>
-      <c r="AO621">
-        <v>0</v>
-      </c>
       <c r="AP621">
-        <v>10</v>
-      </c>
-      <c r="AR621">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AS621">
         <v>0</v>
       </c>
       <c r="AT621">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="AU621">
-        <v>0.05</v>
-      </c>
-      <c r="AW621">
-        <v>0</v>
-      </c>
-      <c r="AX621">
-        <v>0</v>
-      </c>
-      <c r="AY621">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="622" spans="1:51">
@@ -54065,79 +54104,58 @@
         <v>1290</v>
       </c>
       <c r="F622" t="s">
-        <v>1295</v>
+        <v>1317</v>
       </c>
       <c r="K622">
         <v>0</v>
       </c>
       <c r="L622">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="M622">
-        <v>12</v>
+        <v>200</v>
+      </c>
+      <c r="V622">
+        <v>0</v>
+      </c>
+      <c r="W622">
+        <v>0</v>
       </c>
       <c r="Y622">
         <v>1</v>
       </c>
-      <c r="Z622">
-        <v>1</v>
-      </c>
       <c r="AA622">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="AB622">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="AC622" t="s">
         <v>1290</v>
       </c>
-      <c r="AF622">
-        <v>0</v>
-      </c>
-      <c r="AG622">
-        <v>0</v>
-      </c>
-      <c r="AH622">
-        <v>0</v>
-      </c>
-      <c r="AI622">
-        <v>0</v>
-      </c>
-      <c r="AJ622">
-        <v>0</v>
-      </c>
       <c r="AL622">
         <v>1</v>
       </c>
       <c r="AM622">
         <v>1</v>
       </c>
-      <c r="AO622">
-        <v>0</v>
-      </c>
       <c r="AP622">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="AQ622">
+        <v>1</v>
       </c>
       <c r="AR622">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AS622">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT622">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="AU622">
-        <v>0.05</v>
-      </c>
-      <c r="AW622">
-        <v>0</v>
-      </c>
-      <c r="AX622">
-        <v>0</v>
-      </c>
-      <c r="AY622">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="623" spans="1:51">
@@ -54145,52 +54163,55 @@
         <v>1</v>
       </c>
       <c r="D623" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="E623" t="s">
         <v>1290</v>
       </c>
       <c r="F623" t="s">
-        <v>1297</v>
+        <v>1319</v>
       </c>
       <c r="K623">
         <v>0</v>
       </c>
       <c r="L623">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="M623">
-        <v>12</v>
+        <v>300</v>
+      </c>
+      <c r="V623">
+        <v>0</v>
+      </c>
+      <c r="W623">
+        <v>0</v>
       </c>
       <c r="Y623">
         <v>1</v>
       </c>
-      <c r="Z623">
-        <v>1</v>
-      </c>
       <c r="AA623">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="AB623">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="AC623" t="s">
         <v>1290</v>
       </c>
       <c r="AF623">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AG623">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AH623">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AI623">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AJ623">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL623">
         <v>1</v>
@@ -54198,31 +54219,22 @@
       <c r="AM623">
         <v>1</v>
       </c>
-      <c r="AO623">
-        <v>0</v>
-      </c>
       <c r="AP623">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="AQ623">
+        <v>1</v>
       </c>
       <c r="AR623">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AS623">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT623">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="AU623">
-        <v>0.05</v>
-      </c>
-      <c r="AW623">
-        <v>0</v>
-      </c>
-      <c r="AX623">
-        <v>0</v>
-      </c>
-      <c r="AY623">
         <v>0</v>
       </c>
     </row>
@@ -54231,22 +54243,22 @@
         <v>1</v>
       </c>
       <c r="D624" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
       <c r="E624" t="s">
         <v>1290</v>
       </c>
       <c r="F624" t="s">
-        <v>1299</v>
+        <v>1321</v>
       </c>
       <c r="K624">
         <v>0</v>
       </c>
       <c r="L624">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="M624">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="Y624">
         <v>1</v>
@@ -54255,7 +54267,7 @@
         <v>1</v>
       </c>
       <c r="AA624">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB624">
         <v>10</v>
@@ -54290,17 +54302,17 @@
       <c r="AP624">
         <v>10</v>
       </c>
+      <c r="AQ624">
+        <v>1</v>
+      </c>
       <c r="AR624">
-        <v>0</v>
-      </c>
-      <c r="AS624">
-        <v>3</v>
+        <v>0.008</v>
       </c>
       <c r="AT624">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AU624">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AW624">
         <v>0</v>
@@ -54317,13 +54329,13 @@
         <v>1</v>
       </c>
       <c r="D625" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
       <c r="E625" t="s">
         <v>1290</v>
       </c>
       <c r="F625" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
       <c r="K625">
         <v>0</v>
@@ -54380,7 +54392,7 @@
         <v>0</v>
       </c>
       <c r="AS625">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AT625">
         <v>0.05</v>
@@ -54403,13 +54415,13 @@
         <v>1</v>
       </c>
       <c r="D626" t="s">
-        <v>1321</v>
+        <v>1324</v>
       </c>
       <c r="E626" t="s">
         <v>1290</v>
       </c>
       <c r="F626" t="s">
-        <v>1291</v>
+        <v>1295</v>
       </c>
       <c r="K626">
         <v>0</v>
@@ -54445,7 +54457,7 @@
         <v>0</v>
       </c>
       <c r="AI626">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AJ626">
         <v>0</v>
@@ -54466,10 +54478,10 @@
         <v>0</v>
       </c>
       <c r="AS626">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AT626">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AU626">
         <v>0.05</v>
@@ -54489,22 +54501,22 @@
         <v>1</v>
       </c>
       <c r="D627" t="s">
-        <v>1322</v>
+        <v>1325</v>
       </c>
       <c r="E627" t="s">
         <v>1290</v>
       </c>
       <c r="F627" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="K627">
         <v>0</v>
       </c>
       <c r="L627">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="M627">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Y627">
         <v>1</v>
@@ -54513,7 +54525,7 @@
         <v>1</v>
       </c>
       <c r="AA627">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB627">
         <v>10</v>
@@ -54542,20 +54554,23 @@
       <c r="AM627">
         <v>1</v>
       </c>
-      <c r="AN627">
-        <v>1</v>
-      </c>
       <c r="AO627">
+        <v>0</v>
+      </c>
+      <c r="AP627">
+        <v>10</v>
+      </c>
+      <c r="AR627">
+        <v>0</v>
+      </c>
+      <c r="AS627">
+        <v>2</v>
+      </c>
+      <c r="AT627">
         <v>0.05</v>
       </c>
-      <c r="AR627">
-        <v>0</v>
-      </c>
-      <c r="AT627">
-        <v>0</v>
-      </c>
       <c r="AU627">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AW627">
         <v>0</v>
@@ -54572,22 +54587,22 @@
         <v>1</v>
       </c>
       <c r="D628" t="s">
-        <v>1323</v>
+        <v>1326</v>
       </c>
       <c r="E628" t="s">
         <v>1290</v>
       </c>
       <c r="F628" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="K628">
         <v>0</v>
       </c>
       <c r="L628">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M628">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="Y628">
         <v>1</v>
@@ -54596,7 +54611,7 @@
         <v>1</v>
       </c>
       <c r="AA628">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AB628">
         <v>10</v>
@@ -54629,19 +54644,19 @@
         <v>0</v>
       </c>
       <c r="AP628">
-        <v>15</v>
-      </c>
-      <c r="AQ628">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AR628">
-        <v>0.01</v>
+        <v>0</v>
+      </c>
+      <c r="AS628">
+        <v>3</v>
       </c>
       <c r="AT628">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AU628">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AW628">
         <v>0</v>
@@ -54658,22 +54673,22 @@
         <v>1</v>
       </c>
       <c r="D629" t="s">
-        <v>1324</v>
+        <v>1327</v>
       </c>
       <c r="E629" t="s">
         <v>1290</v>
       </c>
       <c r="F629" t="s">
-        <v>1305</v>
+        <v>1328</v>
       </c>
       <c r="K629">
         <v>0</v>
       </c>
       <c r="L629">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="M629">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="Y629">
         <v>1</v>
@@ -54682,7 +54697,7 @@
         <v>1</v>
       </c>
       <c r="AA629">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AB629">
         <v>10</v>
@@ -54715,7 +54730,7 @@
         <v>0</v>
       </c>
       <c r="AP629">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AR629">
         <v>0</v>
@@ -54724,18 +54739,359 @@
         <v>4</v>
       </c>
       <c r="AT629">
+        <v>0.05</v>
+      </c>
+      <c r="AU629">
+        <v>0.05</v>
+      </c>
+      <c r="AW629">
+        <v>0</v>
+      </c>
+      <c r="AX629">
+        <v>0</v>
+      </c>
+      <c r="AY629">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="630" spans="1:51">
+      <c r="C630">
+        <v>1</v>
+      </c>
+      <c r="D630" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E630" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F630" t="s">
+        <v>1291</v>
+      </c>
+      <c r="K630">
+        <v>0</v>
+      </c>
+      <c r="L630">
+        <v>500</v>
+      </c>
+      <c r="M630">
+        <v>12</v>
+      </c>
+      <c r="Y630">
+        <v>1</v>
+      </c>
+      <c r="Z630">
+        <v>1</v>
+      </c>
+      <c r="AA630">
+        <v>3</v>
+      </c>
+      <c r="AB630">
+        <v>10</v>
+      </c>
+      <c r="AC630" t="s">
+        <v>1290</v>
+      </c>
+      <c r="AF630">
+        <v>0</v>
+      </c>
+      <c r="AG630">
+        <v>0</v>
+      </c>
+      <c r="AH630">
+        <v>0</v>
+      </c>
+      <c r="AI630">
+        <v>0.005</v>
+      </c>
+      <c r="AJ630">
+        <v>0</v>
+      </c>
+      <c r="AL630">
+        <v>1</v>
+      </c>
+      <c r="AM630">
+        <v>1</v>
+      </c>
+      <c r="AO630">
+        <v>0</v>
+      </c>
+      <c r="AP630">
+        <v>10</v>
+      </c>
+      <c r="AR630">
+        <v>0</v>
+      </c>
+      <c r="AS630">
+        <v>5</v>
+      </c>
+      <c r="AT630">
+        <v>0</v>
+      </c>
+      <c r="AU630">
+        <v>0.05</v>
+      </c>
+      <c r="AW630">
+        <v>0</v>
+      </c>
+      <c r="AX630">
+        <v>0</v>
+      </c>
+      <c r="AY630">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="631" spans="1:51">
+      <c r="C631">
+        <v>1</v>
+      </c>
+      <c r="D631" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E631" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F631" t="s">
+        <v>1301</v>
+      </c>
+      <c r="K631">
+        <v>0</v>
+      </c>
+      <c r="L631">
+        <v>700</v>
+      </c>
+      <c r="M631">
+        <v>16</v>
+      </c>
+      <c r="Y631">
+        <v>1</v>
+      </c>
+      <c r="Z631">
+        <v>1</v>
+      </c>
+      <c r="AA631">
+        <v>5</v>
+      </c>
+      <c r="AB631">
+        <v>10</v>
+      </c>
+      <c r="AC631" t="s">
+        <v>1290</v>
+      </c>
+      <c r="AF631">
+        <v>0</v>
+      </c>
+      <c r="AG631">
+        <v>0</v>
+      </c>
+      <c r="AH631">
+        <v>0</v>
+      </c>
+      <c r="AI631">
+        <v>0</v>
+      </c>
+      <c r="AJ631">
+        <v>0</v>
+      </c>
+      <c r="AL631">
+        <v>1</v>
+      </c>
+      <c r="AM631">
+        <v>1</v>
+      </c>
+      <c r="AN631">
+        <v>1</v>
+      </c>
+      <c r="AO631">
+        <v>0.05</v>
+      </c>
+      <c r="AR631">
+        <v>0</v>
+      </c>
+      <c r="AT631">
+        <v>0</v>
+      </c>
+      <c r="AU631">
+        <v>0</v>
+      </c>
+      <c r="AW631">
+        <v>0</v>
+      </c>
+      <c r="AX631">
+        <v>0</v>
+      </c>
+      <c r="AY631">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632" spans="1:51">
+      <c r="C632">
+        <v>1</v>
+      </c>
+      <c r="D632" t="s">
+        <v>1331</v>
+      </c>
+      <c r="E632" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F632" t="s">
+        <v>1303</v>
+      </c>
+      <c r="K632">
+        <v>0</v>
+      </c>
+      <c r="L632">
+        <v>1000</v>
+      </c>
+      <c r="M632">
+        <v>20</v>
+      </c>
+      <c r="Y632">
+        <v>1</v>
+      </c>
+      <c r="Z632">
+        <v>1</v>
+      </c>
+      <c r="AA632">
+        <v>8</v>
+      </c>
+      <c r="AB632">
+        <v>10</v>
+      </c>
+      <c r="AC632" t="s">
+        <v>1290</v>
+      </c>
+      <c r="AF632">
+        <v>0</v>
+      </c>
+      <c r="AG632">
+        <v>0</v>
+      </c>
+      <c r="AH632">
+        <v>0</v>
+      </c>
+      <c r="AI632">
+        <v>0</v>
+      </c>
+      <c r="AJ632">
+        <v>0</v>
+      </c>
+      <c r="AL632">
+        <v>1</v>
+      </c>
+      <c r="AM632">
+        <v>1</v>
+      </c>
+      <c r="AO632">
+        <v>0</v>
+      </c>
+      <c r="AP632">
+        <v>15</v>
+      </c>
+      <c r="AQ632">
+        <v>1</v>
+      </c>
+      <c r="AR632">
+        <v>0.01</v>
+      </c>
+      <c r="AT632">
+        <v>0</v>
+      </c>
+      <c r="AU632">
+        <v>0</v>
+      </c>
+      <c r="AW632">
+        <v>0</v>
+      </c>
+      <c r="AX632">
+        <v>0</v>
+      </c>
+      <c r="AY632">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633" spans="1:51">
+      <c r="C633">
+        <v>1</v>
+      </c>
+      <c r="D633" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E633" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F633" t="s">
+        <v>1305</v>
+      </c>
+      <c r="K633">
+        <v>0</v>
+      </c>
+      <c r="L633">
+        <v>2500</v>
+      </c>
+      <c r="M633">
+        <v>24</v>
+      </c>
+      <c r="Y633">
+        <v>1</v>
+      </c>
+      <c r="Z633">
+        <v>1</v>
+      </c>
+      <c r="AA633">
+        <v>10</v>
+      </c>
+      <c r="AB633">
+        <v>10</v>
+      </c>
+      <c r="AC633" t="s">
+        <v>1290</v>
+      </c>
+      <c r="AF633">
+        <v>0</v>
+      </c>
+      <c r="AG633">
+        <v>0</v>
+      </c>
+      <c r="AH633">
+        <v>0</v>
+      </c>
+      <c r="AI633">
+        <v>0</v>
+      </c>
+      <c r="AJ633">
+        <v>0</v>
+      </c>
+      <c r="AL633">
+        <v>1</v>
+      </c>
+      <c r="AM633">
+        <v>1</v>
+      </c>
+      <c r="AO633">
+        <v>0</v>
+      </c>
+      <c r="AP633">
+        <v>15</v>
+      </c>
+      <c r="AR633">
+        <v>0</v>
+      </c>
+      <c r="AS633">
+        <v>4</v>
+      </c>
+      <c r="AT633">
         <v>0.08</v>
       </c>
-      <c r="AU629">
+      <c r="AU633">
         <v>0.08</v>
       </c>
-      <c r="AW629">
-        <v>0</v>
-      </c>
-      <c r="AX629">
-        <v>0</v>
-      </c>
-      <c r="AY629">
+      <c r="AW633">
+        <v>0</v>
+      </c>
+      <c r="AX633">
+        <v>0</v>
+      </c>
+      <c r="AY633">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Broke the import for items into two sets.
- Added a map name value for better checking.
  - Hell wont let our affixes be irrisitible.
  - Hell reduces modded stats by X%.
- Added all items at 400
  - Missing alchemy items and final enchantments.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items.xlsx
+++ b/resources/data-imports/items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42318D50-2352-8A4D-B60E-DA37BF55AE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C9C3AA-925D-B841-B162-7A09B753720F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4423" uniqueCount="2018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4279" uniqueCount="1950">
   <si>
     <t>item_suffix_id</t>
   </si>
@@ -5881,210 +5881,6 @@
   </si>
   <si>
     <t>The power that radiates off this effects this plane in a way I have never seen before. Careful child!</t>
-  </si>
-  <si>
-    <t>Potion of Strength</t>
-  </si>
-  <si>
-    <t>alchemy</t>
-  </si>
-  <si>
-    <t>Adds strength to your character for a limited amount of time</t>
-  </si>
-  <si>
-    <t>Potion of Dexterity</t>
-  </si>
-  <si>
-    <t>Adds dexterity to your character for a limited amount of time</t>
-  </si>
-  <si>
-    <t>Potion of Intelligence</t>
-  </si>
-  <si>
-    <t>Adds intelligence to your character for a limited amount of time</t>
-  </si>
-  <si>
-    <t>Potion of Durability</t>
-  </si>
-  <si>
-    <t>Adds durability to your character for a limited amount of time</t>
-  </si>
-  <si>
-    <t>Potion of Charisma</t>
-  </si>
-  <si>
-    <t>Adds charisma to your character for a limited amount of time</t>
-  </si>
-  <si>
-    <t>Potion of Focus</t>
-  </si>
-  <si>
-    <t>Adds focus to your character for a limited amount of time</t>
-  </si>
-  <si>
-    <t>Potion of Agility</t>
-  </si>
-  <si>
-    <t>Adds agility to your character for a limited amount of time</t>
-  </si>
-  <si>
-    <t>Vial of Impotence</t>
-  </si>
-  <si>
-    <t>Feel the strength coursing through your viens</t>
-  </si>
-  <si>
-    <t>Vial of Shielding</t>
-  </si>
-  <si>
-    <t>Drinking this will cause your base AC by 75% of all training skills.</t>
-  </si>
-  <si>
-    <t>Elixir of Ancient Wisdom</t>
-  </si>
-  <si>
-    <t>Raises your skill attack modifier, intelligence, charisma and focus by 75%.</t>
-  </si>
-  <si>
-    <t>Brew of Lunacy</t>
-  </si>
-  <si>
-    <t>Raises your Skill Attack Modifier by 75%, Strength, Dexterity and Dur by 75%</t>
-  </si>
-  <si>
-    <t>Potion of Moonlight</t>
-  </si>
-  <si>
-    <t>Increases your skill base attack modifier by 75%, your dexterity and agility by 75% as well.</t>
-  </si>
-  <si>
-    <t>Bland Potion</t>
-  </si>
-  <si>
-    <t>This potion tastes bland and gives little effect. But a few of them together ....</t>
-  </si>
-  <si>
-    <t>Training Dust</t>
-  </si>
-  <si>
-    <t>Looking for a boost to those training skills? Now is the time! All your training based skills will get a small boost.</t>
-  </si>
-  <si>
-    <t>Crafters Insight</t>
-  </si>
-  <si>
-    <t>This item will give all your crafting skills a boost!</t>
-  </si>
-  <si>
-    <t>Enchanters Brew</t>
-  </si>
-  <si>
-    <t>Need help with enchanting? Drink a few of these and increase your enchanting chances for a limited time.</t>
-  </si>
-  <si>
-    <t>Disenchanting Powder</t>
-  </si>
-  <si>
-    <t>This power is legit made from the dust from the shards and the gold dust. it will help you disenchant items.</t>
-  </si>
-  <si>
-    <t>Alchemists Drink</t>
-  </si>
-  <si>
-    <t>A drink created by alchemists to help them with their alchemy, I would say this is ingenious.</t>
-  </si>
-  <si>
-    <t>Battle Mages Sand</t>
-  </si>
-  <si>
-    <t>Decrease attack time out by a smidge for a limited time.</t>
-  </si>
-  <si>
-    <t>Time Mages Bomb</t>
-  </si>
-  <si>
-    <t>Blow up a kingdom why don't you. Who doesn't like dropping bombs on kingdoms?</t>
-  </si>
-  <si>
-    <t>Liquid Courage</t>
-  </si>
-  <si>
-    <t>Sometimes you need a boost in battle. Let this be the boost you can rely on!</t>
-  </si>
-  <si>
-    <t>Alchemists Dust</t>
-  </si>
-  <si>
-    <t>A simple dust with a bit of gold dust and the alchemist is full of ideas.</t>
-  </si>
-  <si>
-    <t>Shadow Arch Magi Ink</t>
-  </si>
-  <si>
-    <t>Training Drink</t>
-  </si>
-  <si>
-    <t>Looking for a boost to those training skills? Now is the time! All your training based skills will get a decent boost.</t>
-  </si>
-  <si>
-    <t>Crafters Brew</t>
-  </si>
-  <si>
-    <t>Enchantress Potion</t>
-  </si>
-  <si>
-    <t>Disenchanting Sand</t>
-  </si>
-  <si>
-    <t>Demonic Bomb</t>
-  </si>
-  <si>
-    <t>Demonic Blood</t>
-  </si>
-  <si>
-    <t>Alchemists Eye</t>
-  </si>
-  <si>
-    <t>Astral Mages Ink</t>
-  </si>
-  <si>
-    <t>Enhancement Dust</t>
-  </si>
-  <si>
-    <t>Crafters Crystal Ball</t>
-  </si>
-  <si>
-    <t>Postion of Inspiration</t>
-  </si>
-  <si>
-    <t>Disenchantment Candle</t>
-  </si>
-  <si>
-    <t>Deaths Cloud</t>
-  </si>
-  <si>
-    <t>Quick Feet</t>
-  </si>
-  <si>
-    <t>Move across the land quickly child. The creatures are chasing you.</t>
-  </si>
-  <si>
-    <t>Shattered Shards</t>
-  </si>
-  <si>
-    <t>With this, all your training skills will increase by a % for a specific amount of time.</t>
-  </si>
-  <si>
-    <t>Golden Illusions</t>
-  </si>
-  <si>
-    <t>Create illusions out of gold dust child. These can make you seem stronger and more attuned then you might be.</t>
-  </si>
-  <si>
-    <t>Broken Mirror</t>
-  </si>
-  <si>
-    <t>Look into this broken mirror child. Do you see it? Do you feel it? The strength you need to survive.</t>
   </si>
 </sst>
 </file>
@@ -6424,9 +6220,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD968"/>
+  <dimension ref="A1:BD928"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A907" workbookViewId="0">
+      <selection activeCell="E920" sqref="E920"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -57998,25 +57796,25 @@
         <v>10</v>
       </c>
       <c r="Q546">
-        <v>1.48</v>
+        <v>0.01</v>
       </c>
       <c r="R546">
-        <v>1.48</v>
+        <v>0.01</v>
       </c>
       <c r="S546">
-        <v>1.48</v>
+        <v>0.01</v>
       </c>
       <c r="T546">
-        <v>1.48</v>
+        <v>0.01</v>
       </c>
       <c r="U546">
-        <v>1.48</v>
+        <v>0.01</v>
       </c>
       <c r="V546">
-        <v>1.48</v>
+        <v>0.01</v>
       </c>
       <c r="W546">
-        <v>1.48</v>
+        <v>0.01</v>
       </c>
       <c r="Y546">
         <v>1</v>
@@ -66706,6 +66504,9 @@
       <c r="F636" t="s">
         <v>1357</v>
       </c>
+      <c r="G636" t="s">
+        <v>1283</v>
+      </c>
       <c r="H636">
         <v>1200</v>
       </c>
@@ -66792,6 +66593,9 @@
       <c r="F637" t="s">
         <v>1359</v>
       </c>
+      <c r="G637" t="s">
+        <v>1283</v>
+      </c>
       <c r="H637">
         <v>1300</v>
       </c>
@@ -66887,6 +66691,9 @@
       <c r="F638" t="s">
         <v>1361</v>
       </c>
+      <c r="G638" t="s">
+        <v>1283</v>
+      </c>
       <c r="H638">
         <v>1400</v>
       </c>
@@ -66982,6 +66789,9 @@
       <c r="F639" t="s">
         <v>1363</v>
       </c>
+      <c r="G639" t="s">
+        <v>1283</v>
+      </c>
       <c r="H639">
         <v>1500</v>
       </c>
@@ -67077,6 +66887,9 @@
       <c r="F640" t="s">
         <v>1365</v>
       </c>
+      <c r="G640" t="s">
+        <v>1283</v>
+      </c>
       <c r="H640">
         <v>1600</v>
       </c>
@@ -67172,6 +66985,9 @@
       <c r="F641" t="s">
         <v>1367</v>
       </c>
+      <c r="G641" t="s">
+        <v>1283</v>
+      </c>
       <c r="H641">
         <v>1700</v>
       </c>
@@ -67267,6 +67083,9 @@
       <c r="F642" t="s">
         <v>1369</v>
       </c>
+      <c r="G642" t="s">
+        <v>1283</v>
+      </c>
       <c r="H642">
         <v>1800</v>
       </c>
@@ -67362,6 +67181,9 @@
       <c r="F643" t="s">
         <v>1371</v>
       </c>
+      <c r="G643" t="s">
+        <v>1283</v>
+      </c>
       <c r="H643">
         <v>1900</v>
       </c>
@@ -67448,6 +67270,9 @@
       <c r="F644" t="s">
         <v>1373</v>
       </c>
+      <c r="G644" t="s">
+        <v>1283</v>
+      </c>
       <c r="H644">
         <v>2000</v>
       </c>
@@ -67543,6 +67368,9 @@
       <c r="F645" t="s">
         <v>1375</v>
       </c>
+      <c r="G645" t="s">
+        <v>1283</v>
+      </c>
       <c r="H645">
         <v>2100</v>
       </c>
@@ -67638,6 +67466,9 @@
       <c r="F646" t="s">
         <v>1377</v>
       </c>
+      <c r="G646" t="s">
+        <v>1283</v>
+      </c>
       <c r="H646">
         <v>2200</v>
       </c>
@@ -67733,6 +67564,9 @@
       <c r="F647" t="s">
         <v>1379</v>
       </c>
+      <c r="G647" t="s">
+        <v>1283</v>
+      </c>
       <c r="H647">
         <v>2300</v>
       </c>
@@ -67819,6 +67653,9 @@
       <c r="F648" t="s">
         <v>1381</v>
       </c>
+      <c r="G648" t="s">
+        <v>1283</v>
+      </c>
       <c r="H648">
         <v>2400</v>
       </c>
@@ -67914,6 +67751,9 @@
       <c r="F649" t="s">
         <v>1383</v>
       </c>
+      <c r="G649" t="s">
+        <v>1283</v>
+      </c>
       <c r="H649">
         <v>2500</v>
       </c>
@@ -68021,6 +67861,9 @@
       <c r="F650" t="s">
         <v>1385</v>
       </c>
+      <c r="G650" t="s">
+        <v>1283</v>
+      </c>
       <c r="H650">
         <v>2600</v>
       </c>
@@ -68116,6 +67959,9 @@
       <c r="F651" t="s">
         <v>160</v>
       </c>
+      <c r="G651" t="s">
+        <v>1283</v>
+      </c>
       <c r="H651">
         <v>2700</v>
       </c>
@@ -93872,4010 +93718,6 @@
       </c>
       <c r="BC928">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="929" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C929">
-        <v>1</v>
-      </c>
-      <c r="D929" t="s">
-        <v>1950</v>
-      </c>
-      <c r="E929" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F929" t="s">
-        <v>1952</v>
-      </c>
-      <c r="K929">
-        <v>0</v>
-      </c>
-      <c r="L929">
-        <v>45000</v>
-      </c>
-      <c r="M929">
-        <v>320</v>
-      </c>
-      <c r="Q929">
-        <v>0.35</v>
-      </c>
-      <c r="V929">
-        <v>0</v>
-      </c>
-      <c r="W929">
-        <v>0</v>
-      </c>
-      <c r="Y929">
-        <v>1</v>
-      </c>
-      <c r="AA929">
-        <v>60</v>
-      </c>
-      <c r="AB929">
-        <v>90</v>
-      </c>
-      <c r="AC929" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF929">
-        <v>0</v>
-      </c>
-      <c r="AG929">
-        <v>0</v>
-      </c>
-      <c r="AH929">
-        <v>0</v>
-      </c>
-      <c r="AI929">
-        <v>0</v>
-      </c>
-      <c r="AJ929">
-        <v>0</v>
-      </c>
-      <c r="AL929">
-        <v>1</v>
-      </c>
-      <c r="AM929">
-        <v>1</v>
-      </c>
-      <c r="AO929">
-        <v>0</v>
-      </c>
-      <c r="AP929">
-        <v>15</v>
-      </c>
-      <c r="AR929">
-        <v>0</v>
-      </c>
-      <c r="AT929">
-        <v>0</v>
-      </c>
-      <c r="AU929">
-        <v>0</v>
-      </c>
-      <c r="AW929">
-        <v>0</v>
-      </c>
-      <c r="AX929">
-        <v>0</v>
-      </c>
-      <c r="AY929">
-        <v>0</v>
-      </c>
-      <c r="AZ929">
-        <v>0</v>
-      </c>
-      <c r="BA929">
-        <v>0</v>
-      </c>
-      <c r="BB929">
-        <v>0</v>
-      </c>
-      <c r="BC929">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="930" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C930">
-        <v>1</v>
-      </c>
-      <c r="D930" t="s">
-        <v>1953</v>
-      </c>
-      <c r="E930" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F930" t="s">
-        <v>1954</v>
-      </c>
-      <c r="K930">
-        <v>0</v>
-      </c>
-      <c r="L930">
-        <v>45000</v>
-      </c>
-      <c r="M930">
-        <v>320</v>
-      </c>
-      <c r="S930">
-        <v>0.35</v>
-      </c>
-      <c r="V930">
-        <v>0</v>
-      </c>
-      <c r="W930">
-        <v>0</v>
-      </c>
-      <c r="Y930">
-        <v>1</v>
-      </c>
-      <c r="AA930">
-        <v>60</v>
-      </c>
-      <c r="AB930">
-        <v>90</v>
-      </c>
-      <c r="AC930" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF930">
-        <v>0</v>
-      </c>
-      <c r="AG930">
-        <v>0</v>
-      </c>
-      <c r="AH930">
-        <v>0</v>
-      </c>
-      <c r="AI930">
-        <v>0</v>
-      </c>
-      <c r="AJ930">
-        <v>0</v>
-      </c>
-      <c r="AL930">
-        <v>1</v>
-      </c>
-      <c r="AM930">
-        <v>1</v>
-      </c>
-      <c r="AO930">
-        <v>0</v>
-      </c>
-      <c r="AP930">
-        <v>15</v>
-      </c>
-      <c r="AQ930">
-        <v>1</v>
-      </c>
-      <c r="AR930">
-        <v>0</v>
-      </c>
-      <c r="AT930">
-        <v>0</v>
-      </c>
-      <c r="AU930">
-        <v>0</v>
-      </c>
-      <c r="AW930">
-        <v>0</v>
-      </c>
-      <c r="AX930">
-        <v>0</v>
-      </c>
-      <c r="AY930">
-        <v>0</v>
-      </c>
-      <c r="AZ930">
-        <v>0</v>
-      </c>
-      <c r="BA930">
-        <v>0</v>
-      </c>
-      <c r="BB930">
-        <v>0</v>
-      </c>
-      <c r="BC930">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="931" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C931">
-        <v>1</v>
-      </c>
-      <c r="D931" t="s">
-        <v>1955</v>
-      </c>
-      <c r="E931" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F931" t="s">
-        <v>1956</v>
-      </c>
-      <c r="K931">
-        <v>0</v>
-      </c>
-      <c r="L931">
-        <v>45000</v>
-      </c>
-      <c r="M931">
-        <v>320</v>
-      </c>
-      <c r="U931">
-        <v>0.35</v>
-      </c>
-      <c r="V931">
-        <v>0</v>
-      </c>
-      <c r="W931">
-        <v>0</v>
-      </c>
-      <c r="Y931">
-        <v>1</v>
-      </c>
-      <c r="AA931">
-        <v>60</v>
-      </c>
-      <c r="AB931">
-        <v>90</v>
-      </c>
-      <c r="AC931" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF931">
-        <v>0</v>
-      </c>
-      <c r="AG931">
-        <v>0</v>
-      </c>
-      <c r="AH931">
-        <v>0</v>
-      </c>
-      <c r="AI931">
-        <v>0</v>
-      </c>
-      <c r="AJ931">
-        <v>0</v>
-      </c>
-      <c r="AL931">
-        <v>1</v>
-      </c>
-      <c r="AM931">
-        <v>1</v>
-      </c>
-      <c r="AO931">
-        <v>0</v>
-      </c>
-      <c r="AP931">
-        <v>15</v>
-      </c>
-      <c r="AQ931">
-        <v>1</v>
-      </c>
-      <c r="AR931">
-        <v>0</v>
-      </c>
-      <c r="AT931">
-        <v>0</v>
-      </c>
-      <c r="AU931">
-        <v>0</v>
-      </c>
-      <c r="AW931">
-        <v>0</v>
-      </c>
-      <c r="AX931">
-        <v>0</v>
-      </c>
-      <c r="AY931">
-        <v>0</v>
-      </c>
-      <c r="AZ931">
-        <v>0</v>
-      </c>
-      <c r="BA931">
-        <v>0</v>
-      </c>
-      <c r="BB931">
-        <v>0</v>
-      </c>
-      <c r="BC931">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="932" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C932">
-        <v>1</v>
-      </c>
-      <c r="D932" t="s">
-        <v>1957</v>
-      </c>
-      <c r="E932" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F932" t="s">
-        <v>1958</v>
-      </c>
-      <c r="K932">
-        <v>0</v>
-      </c>
-      <c r="L932">
-        <v>45000</v>
-      </c>
-      <c r="M932">
-        <v>320</v>
-      </c>
-      <c r="R932">
-        <v>0.35</v>
-      </c>
-      <c r="V932">
-        <v>0</v>
-      </c>
-      <c r="W932">
-        <v>0</v>
-      </c>
-      <c r="Y932">
-        <v>1</v>
-      </c>
-      <c r="AA932">
-        <v>60</v>
-      </c>
-      <c r="AB932">
-        <v>90</v>
-      </c>
-      <c r="AC932" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF932">
-        <v>0</v>
-      </c>
-      <c r="AG932">
-        <v>0</v>
-      </c>
-      <c r="AH932">
-        <v>0</v>
-      </c>
-      <c r="AI932">
-        <v>0</v>
-      </c>
-      <c r="AJ932">
-        <v>0</v>
-      </c>
-      <c r="AL932">
-        <v>1</v>
-      </c>
-      <c r="AM932">
-        <v>1</v>
-      </c>
-      <c r="AO932">
-        <v>0</v>
-      </c>
-      <c r="AP932">
-        <v>15</v>
-      </c>
-      <c r="AQ932">
-        <v>1</v>
-      </c>
-      <c r="AR932">
-        <v>0</v>
-      </c>
-      <c r="AT932">
-        <v>0</v>
-      </c>
-      <c r="AU932">
-        <v>0</v>
-      </c>
-      <c r="AW932">
-        <v>0</v>
-      </c>
-      <c r="AX932">
-        <v>0</v>
-      </c>
-      <c r="AY932">
-        <v>0</v>
-      </c>
-      <c r="AZ932">
-        <v>0</v>
-      </c>
-      <c r="BA932">
-        <v>0</v>
-      </c>
-      <c r="BB932">
-        <v>0</v>
-      </c>
-      <c r="BC932">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="933" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C933">
-        <v>1</v>
-      </c>
-      <c r="D933" t="s">
-        <v>1959</v>
-      </c>
-      <c r="E933" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F933" t="s">
-        <v>1960</v>
-      </c>
-      <c r="K933">
-        <v>0</v>
-      </c>
-      <c r="L933">
-        <v>45000</v>
-      </c>
-      <c r="M933">
-        <v>320</v>
-      </c>
-      <c r="T933">
-        <v>0.35</v>
-      </c>
-      <c r="V933">
-        <v>0</v>
-      </c>
-      <c r="W933">
-        <v>0</v>
-      </c>
-      <c r="Y933">
-        <v>1</v>
-      </c>
-      <c r="AA933">
-        <v>60</v>
-      </c>
-      <c r="AB933">
-        <v>90</v>
-      </c>
-      <c r="AC933" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF933">
-        <v>0</v>
-      </c>
-      <c r="AG933">
-        <v>0</v>
-      </c>
-      <c r="AH933">
-        <v>0</v>
-      </c>
-      <c r="AI933">
-        <v>0</v>
-      </c>
-      <c r="AJ933">
-        <v>0</v>
-      </c>
-      <c r="AL933">
-        <v>1</v>
-      </c>
-      <c r="AM933">
-        <v>1</v>
-      </c>
-      <c r="AO933">
-        <v>0</v>
-      </c>
-      <c r="AP933">
-        <v>15</v>
-      </c>
-      <c r="AQ933">
-        <v>1</v>
-      </c>
-      <c r="AR933">
-        <v>0</v>
-      </c>
-      <c r="AW933">
-        <v>0</v>
-      </c>
-      <c r="AX933">
-        <v>0</v>
-      </c>
-      <c r="AY933">
-        <v>0</v>
-      </c>
-      <c r="AZ933">
-        <v>0</v>
-      </c>
-      <c r="BA933">
-        <v>0</v>
-      </c>
-      <c r="BB933">
-        <v>0</v>
-      </c>
-      <c r="BC933">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="934" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C934">
-        <v>1</v>
-      </c>
-      <c r="D934" t="s">
-        <v>1961</v>
-      </c>
-      <c r="E934" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F934" t="s">
-        <v>1962</v>
-      </c>
-      <c r="K934">
-        <v>0</v>
-      </c>
-      <c r="L934">
-        <v>45000</v>
-      </c>
-      <c r="M934">
-        <v>320</v>
-      </c>
-      <c r="V934">
-        <v>0</v>
-      </c>
-      <c r="W934">
-        <v>0.35</v>
-      </c>
-      <c r="Y934">
-        <v>1</v>
-      </c>
-      <c r="AA934">
-        <v>60</v>
-      </c>
-      <c r="AB934">
-        <v>90</v>
-      </c>
-      <c r="AC934" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF934">
-        <v>0</v>
-      </c>
-      <c r="AG934">
-        <v>0</v>
-      </c>
-      <c r="AH934">
-        <v>0</v>
-      </c>
-      <c r="AI934">
-        <v>0</v>
-      </c>
-      <c r="AJ934">
-        <v>0</v>
-      </c>
-      <c r="AL934">
-        <v>1</v>
-      </c>
-      <c r="AM934">
-        <v>1</v>
-      </c>
-      <c r="AO934">
-        <v>0</v>
-      </c>
-      <c r="AP934">
-        <v>15</v>
-      </c>
-      <c r="AQ934">
-        <v>1</v>
-      </c>
-      <c r="AR934">
-        <v>0</v>
-      </c>
-      <c r="AT934">
-        <v>0</v>
-      </c>
-      <c r="AU934">
-        <v>0</v>
-      </c>
-      <c r="AW934">
-        <v>0</v>
-      </c>
-      <c r="AX934">
-        <v>0</v>
-      </c>
-      <c r="AY934">
-        <v>0</v>
-      </c>
-      <c r="AZ934">
-        <v>0</v>
-      </c>
-      <c r="BA934">
-        <v>0</v>
-      </c>
-      <c r="BB934">
-        <v>0</v>
-      </c>
-      <c r="BC934">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="935" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C935">
-        <v>1</v>
-      </c>
-      <c r="D935" t="s">
-        <v>1963</v>
-      </c>
-      <c r="E935" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F935" t="s">
-        <v>1964</v>
-      </c>
-      <c r="K935">
-        <v>0</v>
-      </c>
-      <c r="L935">
-        <v>45000</v>
-      </c>
-      <c r="M935">
-        <v>320</v>
-      </c>
-      <c r="V935">
-        <v>0.35</v>
-      </c>
-      <c r="W935">
-        <v>0</v>
-      </c>
-      <c r="Y935">
-        <v>1</v>
-      </c>
-      <c r="AA935">
-        <v>60</v>
-      </c>
-      <c r="AB935">
-        <v>90</v>
-      </c>
-      <c r="AC935" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF935">
-        <v>0</v>
-      </c>
-      <c r="AG935">
-        <v>0</v>
-      </c>
-      <c r="AH935">
-        <v>0</v>
-      </c>
-      <c r="AI935">
-        <v>0</v>
-      </c>
-      <c r="AJ935">
-        <v>0</v>
-      </c>
-      <c r="AL935">
-        <v>1</v>
-      </c>
-      <c r="AM935">
-        <v>1</v>
-      </c>
-      <c r="AO935">
-        <v>0</v>
-      </c>
-      <c r="AP935">
-        <v>15</v>
-      </c>
-      <c r="AQ935">
-        <v>1</v>
-      </c>
-      <c r="AR935">
-        <v>0</v>
-      </c>
-      <c r="AT935">
-        <v>0</v>
-      </c>
-      <c r="AU935">
-        <v>0</v>
-      </c>
-      <c r="AW935">
-        <v>0</v>
-      </c>
-      <c r="AX935">
-        <v>0</v>
-      </c>
-      <c r="AY935">
-        <v>0</v>
-      </c>
-      <c r="AZ935">
-        <v>0</v>
-      </c>
-      <c r="BA935">
-        <v>0</v>
-      </c>
-      <c r="BB935">
-        <v>0</v>
-      </c>
-      <c r="BC935">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="936" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C936">
-        <v>1</v>
-      </c>
-      <c r="D936" t="s">
-        <v>1965</v>
-      </c>
-      <c r="E936" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F936" t="s">
-        <v>1966</v>
-      </c>
-      <c r="K936">
-        <v>0</v>
-      </c>
-      <c r="L936">
-        <v>50000</v>
-      </c>
-      <c r="M936">
-        <v>380</v>
-      </c>
-      <c r="V936">
-        <v>0</v>
-      </c>
-      <c r="W936">
-        <v>0</v>
-      </c>
-      <c r="Y936">
-        <v>1</v>
-      </c>
-      <c r="AA936">
-        <v>70</v>
-      </c>
-      <c r="AB936">
-        <v>90</v>
-      </c>
-      <c r="AC936" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF936">
-        <v>0.35</v>
-      </c>
-      <c r="AG936">
-        <v>0.35</v>
-      </c>
-      <c r="AH936">
-        <v>0.35</v>
-      </c>
-      <c r="AI936">
-        <v>0</v>
-      </c>
-      <c r="AJ936">
-        <v>0</v>
-      </c>
-      <c r="AL936">
-        <v>1</v>
-      </c>
-      <c r="AM936">
-        <v>1</v>
-      </c>
-      <c r="AO936">
-        <v>0</v>
-      </c>
-      <c r="AP936">
-        <v>30</v>
-      </c>
-      <c r="AQ936">
-        <v>1</v>
-      </c>
-      <c r="AR936">
-        <v>0.6</v>
-      </c>
-      <c r="AS936">
-        <v>0</v>
-      </c>
-      <c r="AT936">
-        <v>0.2</v>
-      </c>
-      <c r="AU936">
-        <v>0.2</v>
-      </c>
-      <c r="AW936">
-        <v>0</v>
-      </c>
-      <c r="AX936">
-        <v>0</v>
-      </c>
-      <c r="AY936">
-        <v>0</v>
-      </c>
-      <c r="AZ936">
-        <v>0</v>
-      </c>
-      <c r="BA936">
-        <v>0</v>
-      </c>
-      <c r="BB936">
-        <v>0</v>
-      </c>
-      <c r="BC936">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="937" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C937">
-        <v>1</v>
-      </c>
-      <c r="D937" t="s">
-        <v>1967</v>
-      </c>
-      <c r="E937" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F937" t="s">
-        <v>1968</v>
-      </c>
-      <c r="K937">
-        <v>0</v>
-      </c>
-      <c r="L937">
-        <v>52000</v>
-      </c>
-      <c r="M937">
-        <v>395</v>
-      </c>
-      <c r="V937">
-        <v>0</v>
-      </c>
-      <c r="W937">
-        <v>0</v>
-      </c>
-      <c r="Y937">
-        <v>1</v>
-      </c>
-      <c r="AA937">
-        <v>80</v>
-      </c>
-      <c r="AB937">
-        <v>90</v>
-      </c>
-      <c r="AC937" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF937">
-        <v>0</v>
-      </c>
-      <c r="AG937">
-        <v>0</v>
-      </c>
-      <c r="AH937">
-        <v>0.75</v>
-      </c>
-      <c r="AI937">
-        <v>0</v>
-      </c>
-      <c r="AJ937">
-        <v>0</v>
-      </c>
-      <c r="AL937">
-        <v>1</v>
-      </c>
-      <c r="AM937">
-        <v>1</v>
-      </c>
-      <c r="AO937">
-        <v>0</v>
-      </c>
-      <c r="AP937">
-        <v>30</v>
-      </c>
-      <c r="AS937">
-        <v>0</v>
-      </c>
-      <c r="AT937">
-        <v>0</v>
-      </c>
-      <c r="AU937">
-        <v>0</v>
-      </c>
-      <c r="AW937">
-        <v>0</v>
-      </c>
-      <c r="AX937">
-        <v>0</v>
-      </c>
-      <c r="AY937">
-        <v>0</v>
-      </c>
-      <c r="AZ937">
-        <v>0</v>
-      </c>
-      <c r="BA937">
-        <v>0</v>
-      </c>
-      <c r="BB937">
-        <v>0</v>
-      </c>
-      <c r="BC937">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="938" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C938">
-        <v>1</v>
-      </c>
-      <c r="D938" t="s">
-        <v>1969</v>
-      </c>
-      <c r="E938" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F938" t="s">
-        <v>1970</v>
-      </c>
-      <c r="K938">
-        <v>0</v>
-      </c>
-      <c r="L938">
-        <v>55000</v>
-      </c>
-      <c r="M938">
-        <v>400</v>
-      </c>
-      <c r="T938">
-        <v>0.75</v>
-      </c>
-      <c r="U938">
-        <v>0.75</v>
-      </c>
-      <c r="V938">
-        <v>0</v>
-      </c>
-      <c r="W938">
-        <v>0.75</v>
-      </c>
-      <c r="Y938">
-        <v>1</v>
-      </c>
-      <c r="AA938">
-        <v>90</v>
-      </c>
-      <c r="AB938">
-        <v>100</v>
-      </c>
-      <c r="AC938" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF938">
-        <v>0.75</v>
-      </c>
-      <c r="AG938">
-        <v>0</v>
-      </c>
-      <c r="AH938">
-        <v>0</v>
-      </c>
-      <c r="AI938">
-        <v>0</v>
-      </c>
-      <c r="AJ938">
-        <v>0</v>
-      </c>
-      <c r="AL938">
-        <v>1</v>
-      </c>
-      <c r="AM938">
-        <v>1</v>
-      </c>
-      <c r="AO938">
-        <v>0</v>
-      </c>
-      <c r="AP938">
-        <v>30</v>
-      </c>
-      <c r="AQ938">
-        <v>1</v>
-      </c>
-      <c r="AR938">
-        <v>0</v>
-      </c>
-      <c r="AS938">
-        <v>0</v>
-      </c>
-      <c r="AT938">
-        <v>0</v>
-      </c>
-      <c r="AU938">
-        <v>0</v>
-      </c>
-      <c r="AW938">
-        <v>0</v>
-      </c>
-      <c r="AX938">
-        <v>0</v>
-      </c>
-      <c r="AY938">
-        <v>0</v>
-      </c>
-      <c r="AZ938">
-        <v>0</v>
-      </c>
-      <c r="BA938">
-        <v>0</v>
-      </c>
-      <c r="BB938">
-        <v>0</v>
-      </c>
-      <c r="BC938">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="939" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C939">
-        <v>1</v>
-      </c>
-      <c r="D939" t="s">
-        <v>1971</v>
-      </c>
-      <c r="E939" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F939" t="s">
-        <v>1972</v>
-      </c>
-      <c r="K939">
-        <v>0</v>
-      </c>
-      <c r="L939">
-        <v>55000</v>
-      </c>
-      <c r="M939">
-        <v>400</v>
-      </c>
-      <c r="Q939">
-        <v>0.75</v>
-      </c>
-      <c r="R939">
-        <v>0.75</v>
-      </c>
-      <c r="S939">
-        <v>0.75</v>
-      </c>
-      <c r="V939">
-        <v>0</v>
-      </c>
-      <c r="W939">
-        <v>0</v>
-      </c>
-      <c r="Y939">
-        <v>1</v>
-      </c>
-      <c r="AA939">
-        <v>100</v>
-      </c>
-      <c r="AB939">
-        <v>110</v>
-      </c>
-      <c r="AC939" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF939">
-        <v>0.75</v>
-      </c>
-      <c r="AG939">
-        <v>0</v>
-      </c>
-      <c r="AH939">
-        <v>0</v>
-      </c>
-      <c r="AI939">
-        <v>0</v>
-      </c>
-      <c r="AJ939">
-        <v>0</v>
-      </c>
-      <c r="AL939">
-        <v>1</v>
-      </c>
-      <c r="AM939">
-        <v>1</v>
-      </c>
-      <c r="AO939">
-        <v>0</v>
-      </c>
-      <c r="AP939">
-        <v>30</v>
-      </c>
-      <c r="AR939">
-        <v>0</v>
-      </c>
-      <c r="AS939">
-        <v>0</v>
-      </c>
-      <c r="AT939">
-        <v>0</v>
-      </c>
-      <c r="AU939">
-        <v>0</v>
-      </c>
-      <c r="AW939">
-        <v>0</v>
-      </c>
-      <c r="AX939">
-        <v>0</v>
-      </c>
-      <c r="AY939">
-        <v>0</v>
-      </c>
-      <c r="AZ939">
-        <v>0</v>
-      </c>
-      <c r="BA939">
-        <v>0</v>
-      </c>
-      <c r="BB939">
-        <v>0</v>
-      </c>
-      <c r="BC939">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="940" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C940">
-        <v>1</v>
-      </c>
-      <c r="D940" t="s">
-        <v>1973</v>
-      </c>
-      <c r="E940" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F940" t="s">
-        <v>1974</v>
-      </c>
-      <c r="K940">
-        <v>0</v>
-      </c>
-      <c r="L940">
-        <v>55000</v>
-      </c>
-      <c r="M940">
-        <v>400</v>
-      </c>
-      <c r="S940">
-        <v>0.75</v>
-      </c>
-      <c r="V940">
-        <v>0.75</v>
-      </c>
-      <c r="W940">
-        <v>0</v>
-      </c>
-      <c r="Y940">
-        <v>1</v>
-      </c>
-      <c r="AA940">
-        <v>120</v>
-      </c>
-      <c r="AB940">
-        <v>130</v>
-      </c>
-      <c r="AC940" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF940">
-        <v>0.75</v>
-      </c>
-      <c r="AG940">
-        <v>0</v>
-      </c>
-      <c r="AH940">
-        <v>0</v>
-      </c>
-      <c r="AI940">
-        <v>0</v>
-      </c>
-      <c r="AJ940">
-        <v>0</v>
-      </c>
-      <c r="AL940">
-        <v>1</v>
-      </c>
-      <c r="AM940">
-        <v>1</v>
-      </c>
-      <c r="AO940">
-        <v>0</v>
-      </c>
-      <c r="AP940">
-        <v>30</v>
-      </c>
-      <c r="AR940">
-        <v>0</v>
-      </c>
-      <c r="AS940">
-        <v>0</v>
-      </c>
-      <c r="AT940">
-        <v>0</v>
-      </c>
-      <c r="AU940">
-        <v>0</v>
-      </c>
-      <c r="AW940">
-        <v>0</v>
-      </c>
-      <c r="AX940">
-        <v>0</v>
-      </c>
-      <c r="AY940">
-        <v>0</v>
-      </c>
-      <c r="AZ940">
-        <v>0</v>
-      </c>
-      <c r="BA940">
-        <v>0</v>
-      </c>
-      <c r="BB940">
-        <v>0</v>
-      </c>
-      <c r="BC940">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="941" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C941">
-        <v>1</v>
-      </c>
-      <c r="D941" t="s">
-        <v>1975</v>
-      </c>
-      <c r="E941" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F941" t="s">
-        <v>1976</v>
-      </c>
-      <c r="K941">
-        <v>0</v>
-      </c>
-      <c r="L941">
-        <v>200</v>
-      </c>
-      <c r="M941">
-        <v>8</v>
-      </c>
-      <c r="Y941">
-        <v>1</v>
-      </c>
-      <c r="Z941">
-        <v>1</v>
-      </c>
-      <c r="AA941">
-        <v>1</v>
-      </c>
-      <c r="AB941">
-        <v>10</v>
-      </c>
-      <c r="AC941" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF941">
-        <v>0</v>
-      </c>
-      <c r="AG941">
-        <v>0</v>
-      </c>
-      <c r="AH941">
-        <v>0</v>
-      </c>
-      <c r="AI941">
-        <v>0</v>
-      </c>
-      <c r="AJ941">
-        <v>0</v>
-      </c>
-      <c r="AL941">
-        <v>1</v>
-      </c>
-      <c r="AM941">
-        <v>1</v>
-      </c>
-      <c r="AO941">
-        <v>0</v>
-      </c>
-      <c r="AP941">
-        <v>10</v>
-      </c>
-      <c r="AQ941">
-        <v>1</v>
-      </c>
-      <c r="AR941">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AT941">
-        <v>0</v>
-      </c>
-      <c r="AU941">
-        <v>0</v>
-      </c>
-      <c r="AW941">
-        <v>0</v>
-      </c>
-      <c r="AX941">
-        <v>0</v>
-      </c>
-      <c r="AY941">
-        <v>0</v>
-      </c>
-      <c r="AZ941">
-        <v>0</v>
-      </c>
-      <c r="BA941">
-        <v>0</v>
-      </c>
-      <c r="BB941">
-        <v>0</v>
-      </c>
-      <c r="BC941">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="942" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C942">
-        <v>1</v>
-      </c>
-      <c r="D942" t="s">
-        <v>1977</v>
-      </c>
-      <c r="E942" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F942" t="s">
-        <v>1978</v>
-      </c>
-      <c r="K942">
-        <v>0</v>
-      </c>
-      <c r="L942">
-        <v>500</v>
-      </c>
-      <c r="M942">
-        <v>12</v>
-      </c>
-      <c r="Y942">
-        <v>1</v>
-      </c>
-      <c r="Z942">
-        <v>1</v>
-      </c>
-      <c r="AA942">
-        <v>3</v>
-      </c>
-      <c r="AB942">
-        <v>10</v>
-      </c>
-      <c r="AC942" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF942">
-        <v>0</v>
-      </c>
-      <c r="AG942">
-        <v>0</v>
-      </c>
-      <c r="AH942">
-        <v>0</v>
-      </c>
-      <c r="AI942">
-        <v>0</v>
-      </c>
-      <c r="AJ942">
-        <v>0</v>
-      </c>
-      <c r="AL942">
-        <v>1</v>
-      </c>
-      <c r="AM942">
-        <v>1</v>
-      </c>
-      <c r="AO942">
-        <v>0</v>
-      </c>
-      <c r="AP942">
-        <v>10</v>
-      </c>
-      <c r="AR942">
-        <v>0</v>
-      </c>
-      <c r="AS942">
-        <v>0</v>
-      </c>
-      <c r="AT942">
-        <v>0.05</v>
-      </c>
-      <c r="AU942">
-        <v>0.05</v>
-      </c>
-      <c r="AW942">
-        <v>0</v>
-      </c>
-      <c r="AX942">
-        <v>0</v>
-      </c>
-      <c r="AY942">
-        <v>0</v>
-      </c>
-      <c r="AZ942">
-        <v>0</v>
-      </c>
-      <c r="BA942">
-        <v>0</v>
-      </c>
-      <c r="BB942">
-        <v>0</v>
-      </c>
-      <c r="BC942">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="943" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C943">
-        <v>1</v>
-      </c>
-      <c r="D943" t="s">
-        <v>1979</v>
-      </c>
-      <c r="E943" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F943" t="s">
-        <v>1980</v>
-      </c>
-      <c r="K943">
-        <v>0</v>
-      </c>
-      <c r="L943">
-        <v>500</v>
-      </c>
-      <c r="M943">
-        <v>12</v>
-      </c>
-      <c r="Y943">
-        <v>1</v>
-      </c>
-      <c r="Z943">
-        <v>1</v>
-      </c>
-      <c r="AA943">
-        <v>3</v>
-      </c>
-      <c r="AB943">
-        <v>10</v>
-      </c>
-      <c r="AC943" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF943">
-        <v>0</v>
-      </c>
-      <c r="AG943">
-        <v>0</v>
-      </c>
-      <c r="AH943">
-        <v>0</v>
-      </c>
-      <c r="AI943">
-        <v>0</v>
-      </c>
-      <c r="AJ943">
-        <v>0</v>
-      </c>
-      <c r="AL943">
-        <v>1</v>
-      </c>
-      <c r="AM943">
-        <v>1</v>
-      </c>
-      <c r="AO943">
-        <v>0</v>
-      </c>
-      <c r="AP943">
-        <v>10</v>
-      </c>
-      <c r="AR943">
-        <v>0</v>
-      </c>
-      <c r="AS943">
-        <v>1</v>
-      </c>
-      <c r="AT943">
-        <v>0.05</v>
-      </c>
-      <c r="AU943">
-        <v>0.05</v>
-      </c>
-      <c r="AW943">
-        <v>0</v>
-      </c>
-      <c r="AX943">
-        <v>0</v>
-      </c>
-      <c r="AY943">
-        <v>0</v>
-      </c>
-      <c r="AZ943">
-        <v>0</v>
-      </c>
-      <c r="BA943">
-        <v>0</v>
-      </c>
-      <c r="BB943">
-        <v>0</v>
-      </c>
-      <c r="BC943">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="944" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C944">
-        <v>1</v>
-      </c>
-      <c r="D944" t="s">
-        <v>1981</v>
-      </c>
-      <c r="E944" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F944" t="s">
-        <v>1982</v>
-      </c>
-      <c r="K944">
-        <v>0</v>
-      </c>
-      <c r="L944">
-        <v>500</v>
-      </c>
-      <c r="M944">
-        <v>12</v>
-      </c>
-      <c r="Y944">
-        <v>1</v>
-      </c>
-      <c r="Z944">
-        <v>1</v>
-      </c>
-      <c r="AA944">
-        <v>3</v>
-      </c>
-      <c r="AB944">
-        <v>10</v>
-      </c>
-      <c r="AC944" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF944">
-        <v>0</v>
-      </c>
-      <c r="AG944">
-        <v>0</v>
-      </c>
-      <c r="AH944">
-        <v>0</v>
-      </c>
-      <c r="AI944">
-        <v>0</v>
-      </c>
-      <c r="AJ944">
-        <v>0</v>
-      </c>
-      <c r="AL944">
-        <v>1</v>
-      </c>
-      <c r="AM944">
-        <v>1</v>
-      </c>
-      <c r="AO944">
-        <v>0</v>
-      </c>
-      <c r="AP944">
-        <v>10</v>
-      </c>
-      <c r="AR944">
-        <v>0</v>
-      </c>
-      <c r="AS944">
-        <v>2</v>
-      </c>
-      <c r="AT944">
-        <v>0.05</v>
-      </c>
-      <c r="AU944">
-        <v>0.05</v>
-      </c>
-      <c r="AW944">
-        <v>0</v>
-      </c>
-      <c r="AX944">
-        <v>0</v>
-      </c>
-      <c r="AY944">
-        <v>0</v>
-      </c>
-      <c r="AZ944">
-        <v>0</v>
-      </c>
-      <c r="BA944">
-        <v>0</v>
-      </c>
-      <c r="BB944">
-        <v>0</v>
-      </c>
-      <c r="BC944">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="945" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C945">
-        <v>1</v>
-      </c>
-      <c r="D945" t="s">
-        <v>1983</v>
-      </c>
-      <c r="E945" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F945" t="s">
-        <v>1984</v>
-      </c>
-      <c r="K945">
-        <v>0</v>
-      </c>
-      <c r="L945">
-        <v>500</v>
-      </c>
-      <c r="M945">
-        <v>12</v>
-      </c>
-      <c r="Y945">
-        <v>1</v>
-      </c>
-      <c r="Z945">
-        <v>1</v>
-      </c>
-      <c r="AA945">
-        <v>3</v>
-      </c>
-      <c r="AB945">
-        <v>10</v>
-      </c>
-      <c r="AC945" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF945">
-        <v>0</v>
-      </c>
-      <c r="AG945">
-        <v>0</v>
-      </c>
-      <c r="AH945">
-        <v>0</v>
-      </c>
-      <c r="AI945">
-        <v>0</v>
-      </c>
-      <c r="AJ945">
-        <v>0</v>
-      </c>
-      <c r="AL945">
-        <v>1</v>
-      </c>
-      <c r="AM945">
-        <v>1</v>
-      </c>
-      <c r="AO945">
-        <v>0</v>
-      </c>
-      <c r="AP945">
-        <v>10</v>
-      </c>
-      <c r="AR945">
-        <v>0</v>
-      </c>
-      <c r="AS945">
-        <v>3</v>
-      </c>
-      <c r="AT945">
-        <v>0.05</v>
-      </c>
-      <c r="AU945">
-        <v>0.05</v>
-      </c>
-      <c r="AW945">
-        <v>0</v>
-      </c>
-      <c r="AX945">
-        <v>0</v>
-      </c>
-      <c r="AY945">
-        <v>0</v>
-      </c>
-      <c r="AZ945">
-        <v>0</v>
-      </c>
-      <c r="BA945">
-        <v>0</v>
-      </c>
-      <c r="BB945">
-        <v>0</v>
-      </c>
-      <c r="BC945">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="946" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C946">
-        <v>1</v>
-      </c>
-      <c r="D946" t="s">
-        <v>1985</v>
-      </c>
-      <c r="E946" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F946" t="s">
-        <v>1986</v>
-      </c>
-      <c r="K946">
-        <v>0</v>
-      </c>
-      <c r="L946">
-        <v>500</v>
-      </c>
-      <c r="M946">
-        <v>12</v>
-      </c>
-      <c r="Y946">
-        <v>1</v>
-      </c>
-      <c r="Z946">
-        <v>1</v>
-      </c>
-      <c r="AA946">
-        <v>3</v>
-      </c>
-      <c r="AB946">
-        <v>10</v>
-      </c>
-      <c r="AC946" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF946">
-        <v>0</v>
-      </c>
-      <c r="AG946">
-        <v>0</v>
-      </c>
-      <c r="AH946">
-        <v>0</v>
-      </c>
-      <c r="AI946">
-        <v>0</v>
-      </c>
-      <c r="AJ946">
-        <v>0</v>
-      </c>
-      <c r="AL946">
-        <v>1</v>
-      </c>
-      <c r="AM946">
-        <v>1</v>
-      </c>
-      <c r="AO946">
-        <v>0</v>
-      </c>
-      <c r="AP946">
-        <v>10</v>
-      </c>
-      <c r="AR946">
-        <v>0</v>
-      </c>
-      <c r="AS946">
-        <v>4</v>
-      </c>
-      <c r="AT946">
-        <v>0.05</v>
-      </c>
-      <c r="AU946">
-        <v>0.05</v>
-      </c>
-      <c r="AW946">
-        <v>0</v>
-      </c>
-      <c r="AX946">
-        <v>0</v>
-      </c>
-      <c r="AY946">
-        <v>0</v>
-      </c>
-      <c r="AZ946">
-        <v>0</v>
-      </c>
-      <c r="BA946">
-        <v>0</v>
-      </c>
-      <c r="BB946">
-        <v>0</v>
-      </c>
-      <c r="BC946">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="947" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C947">
-        <v>1</v>
-      </c>
-      <c r="D947" t="s">
-        <v>1987</v>
-      </c>
-      <c r="E947" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F947" t="s">
-        <v>1988</v>
-      </c>
-      <c r="K947">
-        <v>0</v>
-      </c>
-      <c r="L947">
-        <v>500</v>
-      </c>
-      <c r="M947">
-        <v>12</v>
-      </c>
-      <c r="Y947">
-        <v>1</v>
-      </c>
-      <c r="Z947">
-        <v>1</v>
-      </c>
-      <c r="AA947">
-        <v>3</v>
-      </c>
-      <c r="AB947">
-        <v>10</v>
-      </c>
-      <c r="AC947" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF947">
-        <v>0</v>
-      </c>
-      <c r="AG947">
-        <v>0</v>
-      </c>
-      <c r="AH947">
-        <v>0</v>
-      </c>
-      <c r="AI947">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AJ947">
-        <v>0</v>
-      </c>
-      <c r="AL947">
-        <v>1</v>
-      </c>
-      <c r="AM947">
-        <v>1</v>
-      </c>
-      <c r="AO947">
-        <v>0</v>
-      </c>
-      <c r="AP947">
-        <v>10</v>
-      </c>
-      <c r="AR947">
-        <v>0</v>
-      </c>
-      <c r="AS947">
-        <v>5</v>
-      </c>
-      <c r="AT947">
-        <v>0</v>
-      </c>
-      <c r="AU947">
-        <v>0.05</v>
-      </c>
-      <c r="AW947">
-        <v>0</v>
-      </c>
-      <c r="AX947">
-        <v>0</v>
-      </c>
-      <c r="AY947">
-        <v>0</v>
-      </c>
-      <c r="AZ947">
-        <v>0</v>
-      </c>
-      <c r="BA947">
-        <v>0</v>
-      </c>
-      <c r="BB947">
-        <v>0</v>
-      </c>
-      <c r="BC947">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="948" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C948">
-        <v>1</v>
-      </c>
-      <c r="D948" t="s">
-        <v>1989</v>
-      </c>
-      <c r="E948" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F948" t="s">
-        <v>1990</v>
-      </c>
-      <c r="K948">
-        <v>0</v>
-      </c>
-      <c r="L948">
-        <v>700</v>
-      </c>
-      <c r="M948">
-        <v>16</v>
-      </c>
-      <c r="Y948">
-        <v>1</v>
-      </c>
-      <c r="Z948">
-        <v>1</v>
-      </c>
-      <c r="AA948">
-        <v>5</v>
-      </c>
-      <c r="AB948">
-        <v>10</v>
-      </c>
-      <c r="AC948" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF948">
-        <v>0</v>
-      </c>
-      <c r="AG948">
-        <v>0</v>
-      </c>
-      <c r="AH948">
-        <v>0</v>
-      </c>
-      <c r="AI948">
-        <v>0</v>
-      </c>
-      <c r="AJ948">
-        <v>0</v>
-      </c>
-      <c r="AL948">
-        <v>1</v>
-      </c>
-      <c r="AM948">
-        <v>1</v>
-      </c>
-      <c r="AN948">
-        <v>1</v>
-      </c>
-      <c r="AO948">
-        <v>0.05</v>
-      </c>
-      <c r="AR948">
-        <v>0</v>
-      </c>
-      <c r="AT948">
-        <v>0</v>
-      </c>
-      <c r="AU948">
-        <v>0</v>
-      </c>
-      <c r="AW948">
-        <v>0</v>
-      </c>
-      <c r="AX948">
-        <v>0</v>
-      </c>
-      <c r="AY948">
-        <v>0</v>
-      </c>
-      <c r="AZ948">
-        <v>0</v>
-      </c>
-      <c r="BA948">
-        <v>0</v>
-      </c>
-      <c r="BB948">
-        <v>0</v>
-      </c>
-      <c r="BC948">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="949" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C949">
-        <v>1</v>
-      </c>
-      <c r="D949" t="s">
-        <v>1991</v>
-      </c>
-      <c r="E949" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F949" t="s">
-        <v>1992</v>
-      </c>
-      <c r="K949">
-        <v>0</v>
-      </c>
-      <c r="L949">
-        <v>1000</v>
-      </c>
-      <c r="M949">
-        <v>20</v>
-      </c>
-      <c r="Y949">
-        <v>1</v>
-      </c>
-      <c r="Z949">
-        <v>1</v>
-      </c>
-      <c r="AA949">
-        <v>8</v>
-      </c>
-      <c r="AB949">
-        <v>10</v>
-      </c>
-      <c r="AC949" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF949">
-        <v>0</v>
-      </c>
-      <c r="AG949">
-        <v>0</v>
-      </c>
-      <c r="AH949">
-        <v>0</v>
-      </c>
-      <c r="AI949">
-        <v>0</v>
-      </c>
-      <c r="AJ949">
-        <v>0</v>
-      </c>
-      <c r="AL949">
-        <v>1</v>
-      </c>
-      <c r="AM949">
-        <v>1</v>
-      </c>
-      <c r="AO949">
-        <v>0</v>
-      </c>
-      <c r="AP949">
-        <v>15</v>
-      </c>
-      <c r="AQ949">
-        <v>1</v>
-      </c>
-      <c r="AR949">
-        <v>0.01</v>
-      </c>
-      <c r="AT949">
-        <v>0</v>
-      </c>
-      <c r="AU949">
-        <v>0</v>
-      </c>
-      <c r="AW949">
-        <v>0</v>
-      </c>
-      <c r="AX949">
-        <v>0</v>
-      </c>
-      <c r="AY949">
-        <v>0</v>
-      </c>
-      <c r="AZ949">
-        <v>0</v>
-      </c>
-      <c r="BA949">
-        <v>0</v>
-      </c>
-      <c r="BB949">
-        <v>0</v>
-      </c>
-      <c r="BC949">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="950" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C950">
-        <v>1</v>
-      </c>
-      <c r="D950" t="s">
-        <v>1993</v>
-      </c>
-      <c r="E950" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F950" t="s">
-        <v>1994</v>
-      </c>
-      <c r="K950">
-        <v>0</v>
-      </c>
-      <c r="L950">
-        <v>2500</v>
-      </c>
-      <c r="M950">
-        <v>24</v>
-      </c>
-      <c r="Y950">
-        <v>1</v>
-      </c>
-      <c r="Z950">
-        <v>1</v>
-      </c>
-      <c r="AA950">
-        <v>10</v>
-      </c>
-      <c r="AB950">
-        <v>70</v>
-      </c>
-      <c r="AC950" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF950">
-        <v>0</v>
-      </c>
-      <c r="AG950">
-        <v>0</v>
-      </c>
-      <c r="AH950">
-        <v>0</v>
-      </c>
-      <c r="AI950">
-        <v>0</v>
-      </c>
-      <c r="AJ950">
-        <v>0</v>
-      </c>
-      <c r="AL950">
-        <v>1</v>
-      </c>
-      <c r="AM950">
-        <v>1</v>
-      </c>
-      <c r="AO950">
-        <v>0</v>
-      </c>
-      <c r="AP950">
-        <v>15</v>
-      </c>
-      <c r="AR950">
-        <v>0</v>
-      </c>
-      <c r="AS950">
-        <v>4</v>
-      </c>
-      <c r="AT950">
-        <v>0.08</v>
-      </c>
-      <c r="AU950">
-        <v>0.08</v>
-      </c>
-      <c r="AW950">
-        <v>0</v>
-      </c>
-      <c r="AX950">
-        <v>0</v>
-      </c>
-      <c r="AY950">
-        <v>0</v>
-      </c>
-      <c r="AZ950">
-        <v>0</v>
-      </c>
-      <c r="BA950">
-        <v>0</v>
-      </c>
-      <c r="BB950">
-        <v>0</v>
-      </c>
-      <c r="BC950">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="951" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C951">
-        <v>1</v>
-      </c>
-      <c r="D951" t="s">
-        <v>1995</v>
-      </c>
-      <c r="E951" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F951" t="s">
-        <v>1988</v>
-      </c>
-      <c r="K951">
-        <v>0</v>
-      </c>
-      <c r="L951">
-        <v>2500</v>
-      </c>
-      <c r="M951">
-        <v>24</v>
-      </c>
-      <c r="Y951">
-        <v>1</v>
-      </c>
-      <c r="Z951">
-        <v>1</v>
-      </c>
-      <c r="AA951">
-        <v>10</v>
-      </c>
-      <c r="AB951">
-        <v>70</v>
-      </c>
-      <c r="AC951" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF951">
-        <v>0</v>
-      </c>
-      <c r="AG951">
-        <v>0</v>
-      </c>
-      <c r="AH951">
-        <v>0</v>
-      </c>
-      <c r="AI951">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AJ951">
-        <v>0</v>
-      </c>
-      <c r="AL951">
-        <v>1</v>
-      </c>
-      <c r="AM951">
-        <v>1</v>
-      </c>
-      <c r="AO951">
-        <v>0</v>
-      </c>
-      <c r="AP951">
-        <v>15</v>
-      </c>
-      <c r="AR951">
-        <v>0</v>
-      </c>
-      <c r="AS951">
-        <v>5</v>
-      </c>
-      <c r="AT951">
-        <v>0</v>
-      </c>
-      <c r="AU951">
-        <v>0.08</v>
-      </c>
-      <c r="AW951">
-        <v>0</v>
-      </c>
-      <c r="AX951">
-        <v>0</v>
-      </c>
-      <c r="AY951">
-        <v>0</v>
-      </c>
-      <c r="AZ951">
-        <v>0</v>
-      </c>
-      <c r="BA951">
-        <v>0</v>
-      </c>
-      <c r="BB951">
-        <v>0</v>
-      </c>
-      <c r="BC951">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="952" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C952">
-        <v>1</v>
-      </c>
-      <c r="D952" t="s">
-        <v>1996</v>
-      </c>
-      <c r="E952" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F952" t="s">
-        <v>1997</v>
-      </c>
-      <c r="K952">
-        <v>0</v>
-      </c>
-      <c r="L952">
-        <v>2500</v>
-      </c>
-      <c r="M952">
-        <v>24</v>
-      </c>
-      <c r="Y952">
-        <v>1</v>
-      </c>
-      <c r="Z952">
-        <v>1</v>
-      </c>
-      <c r="AA952">
-        <v>10</v>
-      </c>
-      <c r="AB952">
-        <v>70</v>
-      </c>
-      <c r="AC952" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF952">
-        <v>0</v>
-      </c>
-      <c r="AG952">
-        <v>0</v>
-      </c>
-      <c r="AH952">
-        <v>0</v>
-      </c>
-      <c r="AI952">
-        <v>0</v>
-      </c>
-      <c r="AJ952">
-        <v>0</v>
-      </c>
-      <c r="AL952">
-        <v>1</v>
-      </c>
-      <c r="AM952">
-        <v>1</v>
-      </c>
-      <c r="AO952">
-        <v>0</v>
-      </c>
-      <c r="AP952">
-        <v>15</v>
-      </c>
-      <c r="AR952">
-        <v>0</v>
-      </c>
-      <c r="AS952">
-        <v>0</v>
-      </c>
-      <c r="AT952">
-        <v>0.08</v>
-      </c>
-      <c r="AU952">
-        <v>0.08</v>
-      </c>
-      <c r="AW952">
-        <v>0</v>
-      </c>
-      <c r="AX952">
-        <v>0</v>
-      </c>
-      <c r="AY952">
-        <v>0</v>
-      </c>
-      <c r="AZ952">
-        <v>0</v>
-      </c>
-      <c r="BA952">
-        <v>0</v>
-      </c>
-      <c r="BB952">
-        <v>0</v>
-      </c>
-      <c r="BC952">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="953" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C953">
-        <v>1</v>
-      </c>
-      <c r="D953" t="s">
-        <v>1998</v>
-      </c>
-      <c r="E953" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F953" t="s">
-        <v>1980</v>
-      </c>
-      <c r="K953">
-        <v>0</v>
-      </c>
-      <c r="L953">
-        <v>2500</v>
-      </c>
-      <c r="M953">
-        <v>24</v>
-      </c>
-      <c r="Y953">
-        <v>1</v>
-      </c>
-      <c r="Z953">
-        <v>1</v>
-      </c>
-      <c r="AA953">
-        <v>15</v>
-      </c>
-      <c r="AB953">
-        <v>70</v>
-      </c>
-      <c r="AC953" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF953">
-        <v>0</v>
-      </c>
-      <c r="AG953">
-        <v>0</v>
-      </c>
-      <c r="AH953">
-        <v>0</v>
-      </c>
-      <c r="AI953">
-        <v>0</v>
-      </c>
-      <c r="AJ953">
-        <v>0</v>
-      </c>
-      <c r="AL953">
-        <v>1</v>
-      </c>
-      <c r="AM953">
-        <v>1</v>
-      </c>
-      <c r="AO953">
-        <v>0</v>
-      </c>
-      <c r="AP953">
-        <v>15</v>
-      </c>
-      <c r="AR953">
-        <v>0</v>
-      </c>
-      <c r="AS953">
-        <v>1</v>
-      </c>
-      <c r="AT953">
-        <v>0.08</v>
-      </c>
-      <c r="AU953">
-        <v>0.08</v>
-      </c>
-      <c r="AW953">
-        <v>0</v>
-      </c>
-      <c r="AX953">
-        <v>0</v>
-      </c>
-      <c r="AY953">
-        <v>0</v>
-      </c>
-      <c r="AZ953">
-        <v>0</v>
-      </c>
-      <c r="BA953">
-        <v>0</v>
-      </c>
-      <c r="BB953">
-        <v>0</v>
-      </c>
-      <c r="BC953">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="954" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C954">
-        <v>1</v>
-      </c>
-      <c r="D954" t="s">
-        <v>1999</v>
-      </c>
-      <c r="E954" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F954" t="s">
-        <v>1982</v>
-      </c>
-      <c r="K954">
-        <v>0</v>
-      </c>
-      <c r="L954">
-        <v>2500</v>
-      </c>
-      <c r="M954">
-        <v>24</v>
-      </c>
-      <c r="Y954">
-        <v>1</v>
-      </c>
-      <c r="Z954">
-        <v>1</v>
-      </c>
-      <c r="AA954">
-        <v>15</v>
-      </c>
-      <c r="AB954">
-        <v>70</v>
-      </c>
-      <c r="AC954" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF954">
-        <v>0</v>
-      </c>
-      <c r="AG954">
-        <v>0</v>
-      </c>
-      <c r="AH954">
-        <v>0</v>
-      </c>
-      <c r="AI954">
-        <v>0</v>
-      </c>
-      <c r="AJ954">
-        <v>0</v>
-      </c>
-      <c r="AL954">
-        <v>1</v>
-      </c>
-      <c r="AM954">
-        <v>1</v>
-      </c>
-      <c r="AO954">
-        <v>0</v>
-      </c>
-      <c r="AP954">
-        <v>15</v>
-      </c>
-      <c r="AR954">
-        <v>0</v>
-      </c>
-      <c r="AS954">
-        <v>2</v>
-      </c>
-      <c r="AT954">
-        <v>0.08</v>
-      </c>
-      <c r="AU954">
-        <v>0.08</v>
-      </c>
-      <c r="AW954">
-        <v>0</v>
-      </c>
-      <c r="AX954">
-        <v>0</v>
-      </c>
-      <c r="AY954">
-        <v>0</v>
-      </c>
-      <c r="AZ954">
-        <v>0</v>
-      </c>
-      <c r="BA954">
-        <v>0</v>
-      </c>
-      <c r="BB954">
-        <v>0</v>
-      </c>
-      <c r="BC954">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="955" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C955">
-        <v>1</v>
-      </c>
-      <c r="D955" t="s">
-        <v>2000</v>
-      </c>
-      <c r="E955" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F955" t="s">
-        <v>1984</v>
-      </c>
-      <c r="K955">
-        <v>0</v>
-      </c>
-      <c r="L955">
-        <v>2500</v>
-      </c>
-      <c r="M955">
-        <v>24</v>
-      </c>
-      <c r="Y955">
-        <v>1</v>
-      </c>
-      <c r="Z955">
-        <v>1</v>
-      </c>
-      <c r="AA955">
-        <v>15</v>
-      </c>
-      <c r="AB955">
-        <v>70</v>
-      </c>
-      <c r="AC955" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF955">
-        <v>0</v>
-      </c>
-      <c r="AG955">
-        <v>0</v>
-      </c>
-      <c r="AH955">
-        <v>0</v>
-      </c>
-      <c r="AI955">
-        <v>0</v>
-      </c>
-      <c r="AJ955">
-        <v>0</v>
-      </c>
-      <c r="AL955">
-        <v>1</v>
-      </c>
-      <c r="AM955">
-        <v>1</v>
-      </c>
-      <c r="AO955">
-        <v>0</v>
-      </c>
-      <c r="AP955">
-        <v>15</v>
-      </c>
-      <c r="AR955">
-        <v>0</v>
-      </c>
-      <c r="AS955">
-        <v>3</v>
-      </c>
-      <c r="AT955">
-        <v>0.08</v>
-      </c>
-      <c r="AU955">
-        <v>0.08</v>
-      </c>
-      <c r="AW955">
-        <v>0</v>
-      </c>
-      <c r="AX955">
-        <v>0</v>
-      </c>
-      <c r="AY955">
-        <v>0</v>
-      </c>
-      <c r="AZ955">
-        <v>0</v>
-      </c>
-      <c r="BA955">
-        <v>0</v>
-      </c>
-      <c r="BB955">
-        <v>0</v>
-      </c>
-      <c r="BC955">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="956" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C956">
-        <v>1</v>
-      </c>
-      <c r="D956" t="s">
-        <v>2001</v>
-      </c>
-      <c r="E956" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F956" t="s">
-        <v>1990</v>
-      </c>
-      <c r="K956">
-        <v>0</v>
-      </c>
-      <c r="L956">
-        <v>3000</v>
-      </c>
-      <c r="M956">
-        <v>32</v>
-      </c>
-      <c r="Y956">
-        <v>1</v>
-      </c>
-      <c r="Z956">
-        <v>1</v>
-      </c>
-      <c r="AA956">
-        <v>20</v>
-      </c>
-      <c r="AB956">
-        <v>70</v>
-      </c>
-      <c r="AC956" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF956">
-        <v>0</v>
-      </c>
-      <c r="AG956">
-        <v>0</v>
-      </c>
-      <c r="AH956">
-        <v>0</v>
-      </c>
-      <c r="AI956">
-        <v>0</v>
-      </c>
-      <c r="AJ956">
-        <v>0</v>
-      </c>
-      <c r="AL956">
-        <v>1</v>
-      </c>
-      <c r="AM956">
-        <v>1</v>
-      </c>
-      <c r="AN956">
-        <v>1</v>
-      </c>
-      <c r="AO956">
-        <v>0.08</v>
-      </c>
-      <c r="AR956">
-        <v>0</v>
-      </c>
-      <c r="AT956">
-        <v>0</v>
-      </c>
-      <c r="AU956">
-        <v>0</v>
-      </c>
-      <c r="AW956">
-        <v>0</v>
-      </c>
-      <c r="AX956">
-        <v>0</v>
-      </c>
-      <c r="AY956">
-        <v>0</v>
-      </c>
-      <c r="AZ956">
-        <v>0</v>
-      </c>
-      <c r="BA956">
-        <v>0</v>
-      </c>
-      <c r="BB956">
-        <v>0</v>
-      </c>
-      <c r="BC956">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="957" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C957">
-        <v>1</v>
-      </c>
-      <c r="D957" t="s">
-        <v>2002</v>
-      </c>
-      <c r="E957" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F957" t="s">
-        <v>1992</v>
-      </c>
-      <c r="K957">
-        <v>0</v>
-      </c>
-      <c r="L957">
-        <v>5000</v>
-      </c>
-      <c r="M957">
-        <v>40</v>
-      </c>
-      <c r="Y957">
-        <v>1</v>
-      </c>
-      <c r="Z957">
-        <v>1</v>
-      </c>
-      <c r="AA957">
-        <v>25</v>
-      </c>
-      <c r="AB957">
-        <v>70</v>
-      </c>
-      <c r="AC957" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF957">
-        <v>0</v>
-      </c>
-      <c r="AG957">
-        <v>0</v>
-      </c>
-      <c r="AH957">
-        <v>0</v>
-      </c>
-      <c r="AI957">
-        <v>0</v>
-      </c>
-      <c r="AJ957">
-        <v>0</v>
-      </c>
-      <c r="AL957">
-        <v>1</v>
-      </c>
-      <c r="AM957">
-        <v>1</v>
-      </c>
-      <c r="AO957">
-        <v>0</v>
-      </c>
-      <c r="AP957">
-        <v>20</v>
-      </c>
-      <c r="AQ957">
-        <v>1</v>
-      </c>
-      <c r="AR957">
-        <v>0.05</v>
-      </c>
-      <c r="AT957">
-        <v>0</v>
-      </c>
-      <c r="AU957">
-        <v>0</v>
-      </c>
-      <c r="AW957">
-        <v>0</v>
-      </c>
-      <c r="AX957">
-        <v>0</v>
-      </c>
-      <c r="AY957">
-        <v>0</v>
-      </c>
-      <c r="AZ957">
-        <v>0</v>
-      </c>
-      <c r="BA957">
-        <v>0</v>
-      </c>
-      <c r="BB957">
-        <v>0</v>
-      </c>
-      <c r="BC957">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="958" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C958">
-        <v>1</v>
-      </c>
-      <c r="D958" t="s">
-        <v>2003</v>
-      </c>
-      <c r="E958" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F958" t="s">
-        <v>1994</v>
-      </c>
-      <c r="K958">
-        <v>0</v>
-      </c>
-      <c r="L958">
-        <v>8000</v>
-      </c>
-      <c r="M958">
-        <v>60</v>
-      </c>
-      <c r="Y958">
-        <v>1</v>
-      </c>
-      <c r="Z958">
-        <v>1</v>
-      </c>
-      <c r="AA958">
-        <v>30</v>
-      </c>
-      <c r="AB958">
-        <v>80</v>
-      </c>
-      <c r="AC958" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF958">
-        <v>0</v>
-      </c>
-      <c r="AG958">
-        <v>0</v>
-      </c>
-      <c r="AH958">
-        <v>0</v>
-      </c>
-      <c r="AI958">
-        <v>0</v>
-      </c>
-      <c r="AJ958">
-        <v>0</v>
-      </c>
-      <c r="AL958">
-        <v>1</v>
-      </c>
-      <c r="AM958">
-        <v>1</v>
-      </c>
-      <c r="AO958">
-        <v>0</v>
-      </c>
-      <c r="AP958">
-        <v>20</v>
-      </c>
-      <c r="AR958">
-        <v>0</v>
-      </c>
-      <c r="AS958">
-        <v>4</v>
-      </c>
-      <c r="AT958">
-        <v>0.1</v>
-      </c>
-      <c r="AU958">
-        <v>0.01</v>
-      </c>
-      <c r="AW958">
-        <v>0</v>
-      </c>
-      <c r="AX958">
-        <v>0</v>
-      </c>
-      <c r="AY958">
-        <v>0</v>
-      </c>
-      <c r="AZ958">
-        <v>0</v>
-      </c>
-      <c r="BA958">
-        <v>0</v>
-      </c>
-      <c r="BB958">
-        <v>0</v>
-      </c>
-      <c r="BC958">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="959" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C959">
-        <v>1</v>
-      </c>
-      <c r="D959" t="s">
-        <v>2004</v>
-      </c>
-      <c r="E959" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F959" t="s">
-        <v>1988</v>
-      </c>
-      <c r="K959">
-        <v>0</v>
-      </c>
-      <c r="L959">
-        <v>8000</v>
-      </c>
-      <c r="M959">
-        <v>60</v>
-      </c>
-      <c r="Y959">
-        <v>1</v>
-      </c>
-      <c r="Z959">
-        <v>1</v>
-      </c>
-      <c r="AA959">
-        <v>30</v>
-      </c>
-      <c r="AB959">
-        <v>80</v>
-      </c>
-      <c r="AC959" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF959">
-        <v>0</v>
-      </c>
-      <c r="AG959">
-        <v>0</v>
-      </c>
-      <c r="AH959">
-        <v>0</v>
-      </c>
-      <c r="AI959">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="AJ959">
-        <v>0</v>
-      </c>
-      <c r="AL959">
-        <v>1</v>
-      </c>
-      <c r="AM959">
-        <v>1</v>
-      </c>
-      <c r="AO959">
-        <v>0</v>
-      </c>
-      <c r="AP959">
-        <v>20</v>
-      </c>
-      <c r="AR959">
-        <v>0</v>
-      </c>
-      <c r="AS959">
-        <v>5</v>
-      </c>
-      <c r="AT959">
-        <v>0</v>
-      </c>
-      <c r="AU959">
-        <v>0.01</v>
-      </c>
-      <c r="AW959">
-        <v>0</v>
-      </c>
-      <c r="AX959">
-        <v>0</v>
-      </c>
-      <c r="AY959">
-        <v>0</v>
-      </c>
-      <c r="AZ959">
-        <v>0</v>
-      </c>
-      <c r="BA959">
-        <v>0</v>
-      </c>
-      <c r="BB959">
-        <v>0</v>
-      </c>
-      <c r="BC959">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="960" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C960">
-        <v>1</v>
-      </c>
-      <c r="D960" t="s">
-        <v>2005</v>
-      </c>
-      <c r="E960" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F960" t="s">
-        <v>1997</v>
-      </c>
-      <c r="K960">
-        <v>0</v>
-      </c>
-      <c r="L960">
-        <v>8000</v>
-      </c>
-      <c r="M960">
-        <v>60</v>
-      </c>
-      <c r="Y960">
-        <v>1</v>
-      </c>
-      <c r="Z960">
-        <v>1</v>
-      </c>
-      <c r="AA960">
-        <v>30</v>
-      </c>
-      <c r="AB960">
-        <v>80</v>
-      </c>
-      <c r="AC960" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF960">
-        <v>0</v>
-      </c>
-      <c r="AG960">
-        <v>0</v>
-      </c>
-      <c r="AH960">
-        <v>0</v>
-      </c>
-      <c r="AI960">
-        <v>0</v>
-      </c>
-      <c r="AJ960">
-        <v>0</v>
-      </c>
-      <c r="AL960">
-        <v>1</v>
-      </c>
-      <c r="AM960">
-        <v>1</v>
-      </c>
-      <c r="AO960">
-        <v>0</v>
-      </c>
-      <c r="AP960">
-        <v>20</v>
-      </c>
-      <c r="AR960">
-        <v>0</v>
-      </c>
-      <c r="AS960">
-        <v>0</v>
-      </c>
-      <c r="AT960">
-        <v>0.01</v>
-      </c>
-      <c r="AU960">
-        <v>0.01</v>
-      </c>
-      <c r="AW960">
-        <v>0</v>
-      </c>
-      <c r="AX960">
-        <v>0</v>
-      </c>
-      <c r="AY960">
-        <v>0</v>
-      </c>
-      <c r="AZ960">
-        <v>0</v>
-      </c>
-      <c r="BA960">
-        <v>0</v>
-      </c>
-      <c r="BB960">
-        <v>0</v>
-      </c>
-      <c r="BC960">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="961" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C961">
-        <v>1</v>
-      </c>
-      <c r="D961" t="s">
-        <v>2006</v>
-      </c>
-      <c r="E961" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F961" t="s">
-        <v>1980</v>
-      </c>
-      <c r="K961">
-        <v>0</v>
-      </c>
-      <c r="L961">
-        <v>8000</v>
-      </c>
-      <c r="M961">
-        <v>60</v>
-      </c>
-      <c r="Y961">
-        <v>1</v>
-      </c>
-      <c r="Z961">
-        <v>1</v>
-      </c>
-      <c r="AA961">
-        <v>30</v>
-      </c>
-      <c r="AB961">
-        <v>80</v>
-      </c>
-      <c r="AC961" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF961">
-        <v>0</v>
-      </c>
-      <c r="AG961">
-        <v>0</v>
-      </c>
-      <c r="AH961">
-        <v>0</v>
-      </c>
-      <c r="AI961">
-        <v>0</v>
-      </c>
-      <c r="AJ961">
-        <v>0</v>
-      </c>
-      <c r="AL961">
-        <v>1</v>
-      </c>
-      <c r="AM961">
-        <v>1</v>
-      </c>
-      <c r="AO961">
-        <v>0</v>
-      </c>
-      <c r="AP961">
-        <v>20</v>
-      </c>
-      <c r="AR961">
-        <v>0</v>
-      </c>
-      <c r="AS961">
-        <v>1</v>
-      </c>
-      <c r="AT961">
-        <v>0.01</v>
-      </c>
-      <c r="AU961">
-        <v>0.01</v>
-      </c>
-      <c r="AW961">
-        <v>0</v>
-      </c>
-      <c r="AX961">
-        <v>0</v>
-      </c>
-      <c r="AY961">
-        <v>0</v>
-      </c>
-      <c r="AZ961">
-        <v>0</v>
-      </c>
-      <c r="BA961">
-        <v>0</v>
-      </c>
-      <c r="BB961">
-        <v>0</v>
-      </c>
-      <c r="BC961">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="962" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C962">
-        <v>1</v>
-      </c>
-      <c r="D962" t="s">
-        <v>2007</v>
-      </c>
-      <c r="E962" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F962" t="s">
-        <v>1982</v>
-      </c>
-      <c r="K962">
-        <v>0</v>
-      </c>
-      <c r="L962">
-        <v>8000</v>
-      </c>
-      <c r="M962">
-        <v>60</v>
-      </c>
-      <c r="Y962">
-        <v>1</v>
-      </c>
-      <c r="Z962">
-        <v>1</v>
-      </c>
-      <c r="AA962">
-        <v>30</v>
-      </c>
-      <c r="AB962">
-        <v>80</v>
-      </c>
-      <c r="AC962" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF962">
-        <v>0</v>
-      </c>
-      <c r="AG962">
-        <v>0</v>
-      </c>
-      <c r="AH962">
-        <v>0</v>
-      </c>
-      <c r="AI962">
-        <v>0</v>
-      </c>
-      <c r="AJ962">
-        <v>0</v>
-      </c>
-      <c r="AL962">
-        <v>1</v>
-      </c>
-      <c r="AM962">
-        <v>1</v>
-      </c>
-      <c r="AO962">
-        <v>0</v>
-      </c>
-      <c r="AP962">
-        <v>20</v>
-      </c>
-      <c r="AR962">
-        <v>0</v>
-      </c>
-      <c r="AS962">
-        <v>2</v>
-      </c>
-      <c r="AT962">
-        <v>0.01</v>
-      </c>
-      <c r="AU962">
-        <v>0.01</v>
-      </c>
-      <c r="AW962">
-        <v>0</v>
-      </c>
-      <c r="AX962">
-        <v>0</v>
-      </c>
-      <c r="AY962">
-        <v>0</v>
-      </c>
-      <c r="AZ962">
-        <v>0</v>
-      </c>
-      <c r="BA962">
-        <v>0</v>
-      </c>
-      <c r="BB962">
-        <v>0</v>
-      </c>
-      <c r="BC962">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="963" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C963">
-        <v>1</v>
-      </c>
-      <c r="D963" t="s">
-        <v>2008</v>
-      </c>
-      <c r="E963" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F963" t="s">
-        <v>1984</v>
-      </c>
-      <c r="K963">
-        <v>0</v>
-      </c>
-      <c r="L963">
-        <v>8000</v>
-      </c>
-      <c r="M963">
-        <v>60</v>
-      </c>
-      <c r="Y963">
-        <v>1</v>
-      </c>
-      <c r="Z963">
-        <v>1</v>
-      </c>
-      <c r="AA963">
-        <v>30</v>
-      </c>
-      <c r="AB963">
-        <v>80</v>
-      </c>
-      <c r="AC963" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF963">
-        <v>0</v>
-      </c>
-      <c r="AG963">
-        <v>0</v>
-      </c>
-      <c r="AH963">
-        <v>0</v>
-      </c>
-      <c r="AI963">
-        <v>0</v>
-      </c>
-      <c r="AJ963">
-        <v>0</v>
-      </c>
-      <c r="AL963">
-        <v>1</v>
-      </c>
-      <c r="AM963">
-        <v>1</v>
-      </c>
-      <c r="AO963">
-        <v>0</v>
-      </c>
-      <c r="AP963">
-        <v>20</v>
-      </c>
-      <c r="AR963">
-        <v>0</v>
-      </c>
-      <c r="AS963">
-        <v>3</v>
-      </c>
-      <c r="AT963">
-        <v>0.01</v>
-      </c>
-      <c r="AU963">
-        <v>0.01</v>
-      </c>
-      <c r="AW963">
-        <v>0</v>
-      </c>
-      <c r="AX963">
-        <v>0</v>
-      </c>
-      <c r="AY963">
-        <v>0</v>
-      </c>
-      <c r="AZ963">
-        <v>0</v>
-      </c>
-      <c r="BA963">
-        <v>0</v>
-      </c>
-      <c r="BB963">
-        <v>0</v>
-      </c>
-      <c r="BC963">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="964" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C964">
-        <v>1</v>
-      </c>
-      <c r="D964" t="s">
-        <v>2009</v>
-      </c>
-      <c r="E964" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F964" t="s">
-        <v>1990</v>
-      </c>
-      <c r="K964">
-        <v>0</v>
-      </c>
-      <c r="L964">
-        <v>16000</v>
-      </c>
-      <c r="M964">
-        <v>100</v>
-      </c>
-      <c r="Y964">
-        <v>1</v>
-      </c>
-      <c r="Z964">
-        <v>1</v>
-      </c>
-      <c r="AA964">
-        <v>50</v>
-      </c>
-      <c r="AB964">
-        <v>80</v>
-      </c>
-      <c r="AC964" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF964">
-        <v>0</v>
-      </c>
-      <c r="AG964">
-        <v>0</v>
-      </c>
-      <c r="AH964">
-        <v>0</v>
-      </c>
-      <c r="AI964">
-        <v>0</v>
-      </c>
-      <c r="AJ964">
-        <v>0</v>
-      </c>
-      <c r="AL964">
-        <v>1</v>
-      </c>
-      <c r="AM964">
-        <v>1</v>
-      </c>
-      <c r="AN964">
-        <v>1</v>
-      </c>
-      <c r="AO964">
-        <v>0.1</v>
-      </c>
-      <c r="AR964">
-        <v>0</v>
-      </c>
-      <c r="AT964">
-        <v>0</v>
-      </c>
-      <c r="AU964">
-        <v>0</v>
-      </c>
-      <c r="AW964">
-        <v>0</v>
-      </c>
-      <c r="AX964">
-        <v>0</v>
-      </c>
-      <c r="AY964">
-        <v>0</v>
-      </c>
-      <c r="AZ964">
-        <v>0</v>
-      </c>
-      <c r="BA964">
-        <v>0</v>
-      </c>
-      <c r="BB964">
-        <v>0</v>
-      </c>
-      <c r="BC964">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="965" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C965">
-        <v>1</v>
-      </c>
-      <c r="D965" t="s">
-        <v>2010</v>
-      </c>
-      <c r="E965" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F965" t="s">
-        <v>2011</v>
-      </c>
-      <c r="K965">
-        <v>0</v>
-      </c>
-      <c r="L965">
-        <v>16000</v>
-      </c>
-      <c r="M965">
-        <v>120</v>
-      </c>
-      <c r="V965">
-        <v>0</v>
-      </c>
-      <c r="W965">
-        <v>0</v>
-      </c>
-      <c r="Y965">
-        <v>1</v>
-      </c>
-      <c r="Z965">
-        <v>1</v>
-      </c>
-      <c r="AA965">
-        <v>35</v>
-      </c>
-      <c r="AB965">
-        <v>80</v>
-      </c>
-      <c r="AC965" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF965">
-        <v>0</v>
-      </c>
-      <c r="AG965">
-        <v>0</v>
-      </c>
-      <c r="AH965">
-        <v>0</v>
-      </c>
-      <c r="AI965">
-        <v>0</v>
-      </c>
-      <c r="AJ965">
-        <v>0.03</v>
-      </c>
-      <c r="AL965">
-        <v>1</v>
-      </c>
-      <c r="AM965">
-        <v>1</v>
-      </c>
-      <c r="AO965">
-        <v>0</v>
-      </c>
-      <c r="AP965">
-        <v>22</v>
-      </c>
-      <c r="AR965">
-        <v>0</v>
-      </c>
-      <c r="AS965">
-        <v>6</v>
-      </c>
-      <c r="AT965">
-        <v>0</v>
-      </c>
-      <c r="AU965">
-        <v>0.1</v>
-      </c>
-      <c r="AW965">
-        <v>0</v>
-      </c>
-      <c r="AX965">
-        <v>0</v>
-      </c>
-      <c r="AY965">
-        <v>0</v>
-      </c>
-      <c r="AZ965">
-        <v>0</v>
-      </c>
-      <c r="BA965">
-        <v>0</v>
-      </c>
-      <c r="BB965">
-        <v>0</v>
-      </c>
-      <c r="BC965">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="966" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C966">
-        <v>1</v>
-      </c>
-      <c r="D966" t="s">
-        <v>2012</v>
-      </c>
-      <c r="E966" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F966" t="s">
-        <v>2013</v>
-      </c>
-      <c r="K966">
-        <v>0</v>
-      </c>
-      <c r="L966">
-        <v>18000</v>
-      </c>
-      <c r="M966">
-        <v>150</v>
-      </c>
-      <c r="V966">
-        <v>0</v>
-      </c>
-      <c r="W966">
-        <v>0</v>
-      </c>
-      <c r="Y966">
-        <v>1</v>
-      </c>
-      <c r="Z966">
-        <v>1</v>
-      </c>
-      <c r="AA966">
-        <v>40</v>
-      </c>
-      <c r="AB966">
-        <v>85</v>
-      </c>
-      <c r="AC966" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF966">
-        <v>0.25</v>
-      </c>
-      <c r="AG966">
-        <v>0.25</v>
-      </c>
-      <c r="AH966">
-        <v>0.25</v>
-      </c>
-      <c r="AI966">
-        <v>0.05</v>
-      </c>
-      <c r="AJ966">
-        <v>0.05</v>
-      </c>
-      <c r="AL966">
-        <v>1</v>
-      </c>
-      <c r="AM966">
-        <v>1</v>
-      </c>
-      <c r="AO966">
-        <v>0</v>
-      </c>
-      <c r="AP966">
-        <v>25</v>
-      </c>
-      <c r="AR966">
-        <v>0</v>
-      </c>
-      <c r="AS966">
-        <v>0</v>
-      </c>
-      <c r="AT966">
-        <v>0.25</v>
-      </c>
-      <c r="AU966">
-        <v>0.5</v>
-      </c>
-      <c r="AW966">
-        <v>0</v>
-      </c>
-      <c r="AX966">
-        <v>0</v>
-      </c>
-      <c r="AY966">
-        <v>0</v>
-      </c>
-      <c r="AZ966">
-        <v>0</v>
-      </c>
-      <c r="BA966">
-        <v>0</v>
-      </c>
-      <c r="BB966">
-        <v>0</v>
-      </c>
-      <c r="BC966">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="967" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C967">
-        <v>1</v>
-      </c>
-      <c r="D967" t="s">
-        <v>2014</v>
-      </c>
-      <c r="E967" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F967" t="s">
-        <v>2015</v>
-      </c>
-      <c r="K967">
-        <v>0</v>
-      </c>
-      <c r="L967">
-        <v>20000</v>
-      </c>
-      <c r="M967">
-        <v>200</v>
-      </c>
-      <c r="V967">
-        <v>0</v>
-      </c>
-      <c r="W967">
-        <v>0</v>
-      </c>
-      <c r="Y967">
-        <v>1</v>
-      </c>
-      <c r="Z967">
-        <v>1</v>
-      </c>
-      <c r="AA967">
-        <v>45</v>
-      </c>
-      <c r="AB967">
-        <v>90</v>
-      </c>
-      <c r="AC967" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF967">
-        <v>0</v>
-      </c>
-      <c r="AG967">
-        <v>0</v>
-      </c>
-      <c r="AH967">
-        <v>0</v>
-      </c>
-      <c r="AI967">
-        <v>0</v>
-      </c>
-      <c r="AJ967">
-        <v>0</v>
-      </c>
-      <c r="AL967">
-        <v>1</v>
-      </c>
-      <c r="AM967">
-        <v>1</v>
-      </c>
-      <c r="AO967">
-        <v>0</v>
-      </c>
-      <c r="AP967">
-        <v>28</v>
-      </c>
-      <c r="AQ967">
-        <v>1</v>
-      </c>
-      <c r="AR967">
-        <v>0.1</v>
-      </c>
-      <c r="AS967">
-        <v>3</v>
-      </c>
-      <c r="AT967">
-        <v>0.15</v>
-      </c>
-      <c r="AU967">
-        <v>0.25</v>
-      </c>
-      <c r="AW967">
-        <v>0</v>
-      </c>
-      <c r="AX967">
-        <v>0</v>
-      </c>
-      <c r="AY967">
-        <v>0</v>
-      </c>
-      <c r="AZ967">
-        <v>0</v>
-      </c>
-      <c r="BA967">
-        <v>0</v>
-      </c>
-      <c r="BB967">
-        <v>0</v>
-      </c>
-      <c r="BC967">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="968" spans="3:55" x14ac:dyDescent="0.2">
-      <c r="C968">
-        <v>1</v>
-      </c>
-      <c r="D968" t="s">
-        <v>2016</v>
-      </c>
-      <c r="E968" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F968" t="s">
-        <v>2017</v>
-      </c>
-      <c r="K968">
-        <v>0</v>
-      </c>
-      <c r="L968">
-        <v>21000</v>
-      </c>
-      <c r="M968">
-        <v>300</v>
-      </c>
-      <c r="V968">
-        <v>0</v>
-      </c>
-      <c r="W968">
-        <v>0</v>
-      </c>
-      <c r="Y968">
-        <v>1</v>
-      </c>
-      <c r="Z968">
-        <v>1</v>
-      </c>
-      <c r="AA968">
-        <v>50</v>
-      </c>
-      <c r="AB968">
-        <v>90</v>
-      </c>
-      <c r="AC968" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AF968">
-        <v>0.5</v>
-      </c>
-      <c r="AG968">
-        <v>0.5</v>
-      </c>
-      <c r="AH968">
-        <v>0.5</v>
-      </c>
-      <c r="AI968">
-        <v>0.5</v>
-      </c>
-      <c r="AJ968">
-        <v>0.5</v>
-      </c>
-      <c r="AL968">
-        <v>1</v>
-      </c>
-      <c r="AM968">
-        <v>1</v>
-      </c>
-      <c r="AO968">
-        <v>0</v>
-      </c>
-      <c r="AP968">
-        <v>30</v>
-      </c>
-      <c r="AQ968">
-        <v>1</v>
-      </c>
-      <c r="AR968">
-        <v>0.15</v>
-      </c>
-      <c r="AS968">
-        <v>0</v>
-      </c>
-      <c r="AT968">
-        <v>0.5</v>
-      </c>
-      <c r="AU968">
-        <v>0</v>
-      </c>
-      <c r="AW968">
-        <v>0</v>
-      </c>
-      <c r="AX968">
-        <v>0</v>
-      </c>
-      <c r="AY968">
-        <v>0</v>
-      </c>
-      <c r="AZ968">
-        <v>0</v>
-      </c>
-      <c r="BA968">
-        <v>0</v>
-      </c>
-      <c r="BB968">
-        <v>0</v>
-      </c>
-      <c r="BC968">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>